<commit_message>
M3 QA Cord #326 - Implements Cord Test Data #286   - Implement import UnitTest.TensileStrength #18
</commit_message>
<xml_diff>
--- a/05.Controls/M3.QA.Controls/Resources/Excels/COA1.xlsx
+++ b/05.Controls/M3.QA.Controls/Resources/Excels/COA1.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="46">
   <si>
     <t>Toray Textiles (Thailand) Public Company Limited  Mill 3</t>
   </si>
@@ -152,9 +152,6 @@
     <t>(N)</t>
   </si>
   <si>
-    <t>OK</t>
-  </si>
-  <si>
     <t>ELONG. AT BREAK</t>
   </si>
   <si>
@@ -219,7 +216,7 @@
     <numFmt numFmtId="166" formatCode="[$-1010409]d\ mmm\ yy;@"/>
     <numFmt numFmtId="167" formatCode="0.0"/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -351,6 +348,12 @@
       <color rgb="FFFF0000"/>
       <name val="AngsanaUPC"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <name val="AngsanaUPC"/>
+      <family val="1"/>
+      <charset val="222"/>
     </font>
   </fonts>
   <fills count="2">
@@ -601,30 +604,12 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="4" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
@@ -762,6 +747,48 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -798,47 +825,23 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="11">
@@ -907,7 +910,7 @@
         <xdr:cNvPr id="2" name="Picture 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8C6984C9-0C37-400A-AFFE-0753047B13B4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{8C6984C9-0C37-400A-AFFE-0753047B13B4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1233,7 +1236,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1244,7 +1247,7 @@
   <dimension ref="A1:Y36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23:F23"/>
+      <selection activeCell="E12" sqref="E12:H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.5546875" defaultRowHeight="13.2"/>
@@ -1257,7 +1260,7 @@
     <col min="10" max="13" width="7.5546875" style="2"/>
     <col min="14" max="14" width="10.44140625" style="2" customWidth="1"/>
     <col min="15" max="24" width="7.5546875" style="2"/>
-    <col min="25" max="25" width="7.5546875" style="53"/>
+    <col min="25" max="25" width="7.5546875" style="47"/>
     <col min="26" max="16384" width="7.5546875" style="2"/>
   </cols>
   <sheetData>
@@ -1271,7 +1274,7 @@
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
-      <c r="N1" s="98"/>
+      <c r="N1" s="73"/>
     </row>
     <row r="2" spans="1:23" ht="14.25" customHeight="1">
       <c r="A2" s="3" t="s">
@@ -1285,7 +1288,7 @@
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
-      <c r="N2" s="99"/>
+      <c r="N2" s="74"/>
     </row>
     <row r="3" spans="1:23" ht="14.25" customHeight="1">
       <c r="A3" s="3" t="s">
@@ -1299,7 +1302,7 @@
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
-      <c r="N3" s="99"/>
+      <c r="N3" s="74"/>
     </row>
     <row r="4" spans="1:23" ht="14.25" customHeight="1">
       <c r="A4" s="3" t="s">
@@ -1313,7 +1316,7 @@
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
-      <c r="N4" s="99"/>
+      <c r="N4" s="74"/>
       <c r="W4" s="4"/>
     </row>
     <row r="5" spans="1:23" ht="14.25" customHeight="1">
@@ -1328,7 +1331,7 @@
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
-      <c r="N5" s="99"/>
+      <c r="N5" s="74"/>
     </row>
     <row r="6" spans="1:23" ht="14.25" customHeight="1">
       <c r="A6" s="5" t="s">
@@ -1342,7 +1345,7 @@
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
-      <c r="N6" s="99"/>
+      <c r="N6" s="74"/>
     </row>
     <row r="7" spans="1:23" ht="20.399999999999999">
       <c r="A7" s="5"/>
@@ -1361,7 +1364,7 @@
       <c r="J7" s="9"/>
       <c r="K7" s="9"/>
       <c r="L7" s="9"/>
-      <c r="N7" s="99"/>
+      <c r="N7" s="74"/>
     </row>
     <row r="8" spans="1:23" ht="19.8">
       <c r="A8" s="1"/>
@@ -1373,7 +1376,7 @@
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
-      <c r="N8" s="99"/>
+      <c r="N8" s="74"/>
     </row>
     <row r="9" spans="1:23" ht="26.4">
       <c r="A9" s="10" t="s">
@@ -1387,7 +1390,7 @@
       <c r="G9" s="6"/>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
-      <c r="N9" s="100"/>
+      <c r="N9" s="75"/>
     </row>
     <row r="10" spans="1:23" ht="19.8">
       <c r="A10" s="1"/>
@@ -1401,7 +1404,7 @@
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
-      <c r="N10" s="99"/>
+      <c r="N10" s="74"/>
     </row>
     <row r="11" spans="1:23" ht="22.5" customHeight="1">
       <c r="A11" s="13" t="s">
@@ -1419,7 +1422,7 @@
       <c r="I11" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="N11" s="99"/>
+      <c r="N11" s="74"/>
     </row>
     <row r="12" spans="1:23" ht="22.5" customHeight="1">
       <c r="A12" s="13" t="s">
@@ -1428,104 +1431,77 @@
       <c r="B12" s="19"/>
       <c r="C12" s="13"/>
       <c r="D12" s="13"/>
-      <c r="E12" s="20" t="str">
-        <f>+IF(G20=M20,+"","NO PASSED")</f>
-        <v>NO PASSED</v>
-      </c>
-      <c r="F12" s="21" t="str">
-        <f>+IF(G22=M22,+"","NO PASSED")</f>
-        <v>NO PASSED</v>
-      </c>
-      <c r="G12" s="21"/>
-      <c r="H12" s="22" t="str">
-        <f>+IF(G24=M24,+"","NO PASSED")</f>
-        <v>NO PASSED</v>
-      </c>
-      <c r="I12" s="23" t="str">
-        <f>+IF(G26=M26,+"","NO PASSED")</f>
-        <v>NO PASSED</v>
-      </c>
-      <c r="N12" s="99"/>
+      <c r="E12" s="99"/>
+      <c r="F12" s="100"/>
+      <c r="G12" s="100"/>
+      <c r="H12" s="101"/>
+      <c r="I12" s="20"/>
+      <c r="N12" s="74"/>
     </row>
     <row r="13" spans="1:23" ht="22.5" customHeight="1">
       <c r="A13" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="24"/>
-      <c r="C13" s="25"/>
+      <c r="B13" s="21"/>
+      <c r="C13" s="22"/>
       <c r="D13" s="13"/>
-      <c r="E13" s="26" t="str">
-        <f>+IF(G21=M21,+"","NO PASSED")</f>
-        <v>NO PASSED</v>
-      </c>
-      <c r="F13" s="27" t="str">
-        <f>+IF(G23=M23,+"","NO PASSED")</f>
-        <v>NO PASSED</v>
-      </c>
-      <c r="G13" s="27"/>
-      <c r="H13" s="28" t="str">
-        <f>+IF(G25=M25,+"","NO PASSED")</f>
-        <v>NO PASSED</v>
-      </c>
-      <c r="I13" s="23" t="str">
-        <f>+IF(G27=M27,+"","NO PASSED")</f>
-        <v>NO PASSED</v>
-      </c>
-      <c r="K13" s="29"/>
-      <c r="N13" s="99"/>
+      <c r="E13" s="102"/>
+      <c r="F13" s="103"/>
+      <c r="G13" s="103"/>
+      <c r="H13" s="104"/>
+      <c r="I13" s="20"/>
+      <c r="K13" s="23"/>
+      <c r="N13" s="74"/>
     </row>
     <row r="14" spans="1:23" ht="22.5" customHeight="1">
       <c r="A14" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="30"/>
+      <c r="B14" s="24"/>
       <c r="C14" s="13"/>
       <c r="D14" s="13"/>
-      <c r="E14" s="79" t="s">
+      <c r="E14" s="87" t="s">
         <v>13</v>
       </c>
-      <c r="F14" s="80"/>
-      <c r="G14" s="79" t="s">
+      <c r="F14" s="88"/>
+      <c r="G14" s="87" t="s">
         <v>14</v>
       </c>
-      <c r="H14" s="80"/>
-      <c r="I14" s="31" t="s">
+      <c r="H14" s="88"/>
+      <c r="I14" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="N14" s="99"/>
+      <c r="N14" s="74"/>
     </row>
     <row r="15" spans="1:23" ht="22.5" customHeight="1">
       <c r="A15" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="81"/>
-      <c r="C15" s="81"/>
+      <c r="B15" s="89"/>
+      <c r="C15" s="89"/>
       <c r="D15" s="13"/>
-      <c r="E15" s="32"/>
-      <c r="F15" s="33"/>
-      <c r="G15" s="32"/>
-      <c r="H15" s="34"/>
-      <c r="I15" s="23" t="str">
-        <f>+IF(G28=M28,+"","NO PASSED")</f>
-        <v>NO PASSED</v>
-      </c>
-      <c r="N15" s="99"/>
+      <c r="E15" s="26"/>
+      <c r="F15" s="27"/>
+      <c r="G15" s="26"/>
+      <c r="H15" s="28"/>
+      <c r="I15" s="20"/>
+      <c r="N15" s="74"/>
     </row>
     <row r="16" spans="1:23" ht="22.5" customHeight="1">
       <c r="A16" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="35"/>
-      <c r="C16" s="30" t="s">
+      <c r="B16" s="29"/>
+      <c r="C16" s="24" t="s">
         <v>18</v>
       </c>
       <c r="D16" s="13"/>
-      <c r="E16" s="36"/>
-      <c r="F16" s="37"/>
-      <c r="G16" s="36"/>
-      <c r="H16" s="38"/>
-      <c r="I16" s="39"/>
-      <c r="N16" s="99"/>
+      <c r="E16" s="30"/>
+      <c r="F16" s="31"/>
+      <c r="G16" s="30"/>
+      <c r="H16" s="32"/>
+      <c r="I16" s="33"/>
+      <c r="N16" s="74"/>
     </row>
     <row r="17" spans="1:25" ht="19.8">
       <c r="A17" s="1" t="s">
@@ -1539,344 +1515,324 @@
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
-      <c r="N17" s="99"/>
-      <c r="Y17" s="82"/>
+      <c r="N17" s="74"/>
+      <c r="Y17" s="90"/>
     </row>
     <row r="18" spans="1:25" ht="19.8">
-      <c r="A18" s="83" t="s">
+      <c r="A18" s="91" t="s">
         <v>20</v>
       </c>
-      <c r="B18" s="84"/>
-      <c r="C18" s="85"/>
-      <c r="D18" s="89" t="s">
+      <c r="B18" s="92"/>
+      <c r="C18" s="93"/>
+      <c r="D18" s="97" t="s">
         <v>21</v>
       </c>
-      <c r="E18" s="83" t="s">
+      <c r="E18" s="91" t="s">
         <v>22</v>
       </c>
-      <c r="F18" s="85"/>
-      <c r="G18" s="89" t="s">
+      <c r="F18" s="93"/>
+      <c r="G18" s="97" t="s">
         <v>23</v>
       </c>
-      <c r="H18" s="40" t="s">
+      <c r="H18" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="I18" s="41"/>
-      <c r="N18" s="99"/>
+      <c r="I18" s="35"/>
+      <c r="N18" s="74"/>
       <c r="Q18" s="13"/>
-      <c r="T18" s="42"/>
-      <c r="Y18" s="82"/>
+      <c r="T18" s="36"/>
+      <c r="Y18" s="90"/>
     </row>
     <row r="19" spans="1:25" ht="21.6">
-      <c r="A19" s="86"/>
-      <c r="B19" s="87"/>
-      <c r="C19" s="88"/>
-      <c r="D19" s="90"/>
-      <c r="E19" s="86"/>
-      <c r="F19" s="88"/>
-      <c r="G19" s="90"/>
-      <c r="H19" s="43" t="s">
+      <c r="A19" s="94"/>
+      <c r="B19" s="95"/>
+      <c r="C19" s="96"/>
+      <c r="D19" s="98"/>
+      <c r="E19" s="94"/>
+      <c r="F19" s="96"/>
+      <c r="G19" s="98"/>
+      <c r="H19" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="I19" s="44"/>
-      <c r="K19" s="29"/>
-      <c r="L19" s="29"/>
-      <c r="M19" s="29"/>
+      <c r="I19" s="38"/>
+      <c r="K19" s="23"/>
+      <c r="L19" s="23"/>
+      <c r="M19" s="23"/>
       <c r="Q19" s="13"/>
-      <c r="T19" s="42"/>
-      <c r="Y19" s="82"/>
+      <c r="T19" s="36"/>
+      <c r="Y19" s="90"/>
     </row>
     <row r="20" spans="1:25" ht="19.8">
-      <c r="A20" s="45" t="s">
+      <c r="A20" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="B20" s="46"/>
-      <c r="C20" s="47" t="s">
+      <c r="B20" s="40"/>
+      <c r="C20" s="41" t="s">
         <v>27</v>
       </c>
-      <c r="D20" s="48"/>
-      <c r="E20" s="101"/>
-      <c r="F20" s="102"/>
-      <c r="G20" s="49"/>
-      <c r="H20" s="92"/>
-      <c r="I20" s="93"/>
-      <c r="K20" s="50">
+      <c r="D20" s="42"/>
+      <c r="E20" s="76"/>
+      <c r="F20" s="77"/>
+      <c r="G20" s="43"/>
+      <c r="H20" s="83"/>
+      <c r="I20" s="84"/>
+      <c r="K20" s="44">
         <v>136</v>
       </c>
-      <c r="L20" s="50">
+      <c r="L20" s="44">
         <v>180</v>
       </c>
-      <c r="M20" s="51" t="s">
+      <c r="M20" s="45"/>
+      <c r="Q20" s="13"/>
+      <c r="T20" s="46"/>
+    </row>
+    <row r="21" spans="1:25" ht="19.8">
+      <c r="A21" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="Q20" s="13"/>
-      <c r="T20" s="52"/>
-    </row>
-    <row r="21" spans="1:25" ht="19.8">
-      <c r="A21" s="45" t="s">
+      <c r="B21" s="40"/>
+      <c r="C21" s="41" t="s">
         <v>29</v>
       </c>
-      <c r="B21" s="46"/>
-      <c r="C21" s="47" t="s">
+      <c r="D21" s="48"/>
+      <c r="E21" s="76"/>
+      <c r="F21" s="77"/>
+      <c r="G21" s="43"/>
+      <c r="H21" s="83"/>
+      <c r="I21" s="84"/>
+      <c r="K21" s="44">
+        <v>11</v>
+      </c>
+      <c r="L21" s="44">
+        <v>18</v>
+      </c>
+      <c r="M21" s="45"/>
+      <c r="Q21" s="1"/>
+      <c r="T21" s="49"/>
+      <c r="Y21" s="50"/>
+    </row>
+    <row r="22" spans="1:25" ht="19.8">
+      <c r="A22" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="D21" s="54"/>
-      <c r="E21" s="101"/>
-      <c r="F21" s="102"/>
-      <c r="G21" s="49"/>
-      <c r="H21" s="92"/>
-      <c r="I21" s="93"/>
-      <c r="K21" s="50">
-        <v>11</v>
-      </c>
-      <c r="L21" s="50">
-        <v>18</v>
-      </c>
-      <c r="M21" s="51" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q21" s="1"/>
-      <c r="T21" s="55"/>
-      <c r="Y21" s="56"/>
-    </row>
-    <row r="22" spans="1:25" ht="19.8">
-      <c r="A22" s="45" t="s">
+      <c r="B22" s="40"/>
+      <c r="C22" s="41" t="s">
+        <v>29</v>
+      </c>
+      <c r="D22" s="51"/>
+      <c r="E22" s="76"/>
+      <c r="F22" s="77"/>
+      <c r="G22" s="52"/>
+      <c r="H22" s="83"/>
+      <c r="I22" s="84"/>
+      <c r="K22" s="44">
+        <v>1.99</v>
+      </c>
+      <c r="L22" s="44">
+        <v>4.99</v>
+      </c>
+      <c r="M22" s="45"/>
+      <c r="Q22" s="1"/>
+      <c r="Y22" s="49"/>
+    </row>
+    <row r="23" spans="1:25" ht="24.75" customHeight="1">
+      <c r="A23" s="53" t="s">
         <v>31</v>
       </c>
-      <c r="B22" s="46"/>
-      <c r="C22" s="47" t="s">
-        <v>30</v>
-      </c>
-      <c r="D22" s="57"/>
-      <c r="E22" s="101"/>
-      <c r="F22" s="102"/>
-      <c r="G22" s="58"/>
-      <c r="H22" s="92"/>
-      <c r="I22" s="93"/>
-      <c r="K22" s="50">
-        <v>1.99</v>
-      </c>
-      <c r="L22" s="50">
-        <v>4.99</v>
-      </c>
-      <c r="M22" s="51" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q22" s="1"/>
-      <c r="Y22" s="55"/>
-    </row>
-    <row r="23" spans="1:25" ht="24.75" customHeight="1">
-      <c r="A23" s="59" t="s">
+      <c r="B23" s="1"/>
+      <c r="C23" s="54" t="s">
         <v>32</v>
       </c>
-      <c r="B23" s="1"/>
-      <c r="C23" s="60" t="s">
+      <c r="D23" s="55"/>
+      <c r="E23" s="76"/>
+      <c r="F23" s="77"/>
+      <c r="G23" s="52"/>
+      <c r="H23" s="83"/>
+      <c r="I23" s="84"/>
+      <c r="K23" s="44">
+        <v>10.49</v>
+      </c>
+      <c r="L23" s="44">
+        <v>12.49</v>
+      </c>
+      <c r="M23" s="45"/>
+      <c r="Q23" s="13"/>
+    </row>
+    <row r="24" spans="1:25" ht="19.8">
+      <c r="A24" s="56" t="s">
         <v>33</v>
       </c>
-      <c r="D23" s="61"/>
-      <c r="E23" s="101"/>
-      <c r="F23" s="102"/>
-      <c r="G23" s="58"/>
-      <c r="H23" s="92"/>
-      <c r="I23" s="93"/>
-      <c r="K23" s="50">
-        <v>10.49</v>
-      </c>
-      <c r="L23" s="50">
-        <v>12.49</v>
-      </c>
-      <c r="M23" s="51" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q23" s="13"/>
-    </row>
-    <row r="24" spans="1:25" ht="19.8">
-      <c r="A24" s="62" t="s">
+      <c r="B24" s="57"/>
+      <c r="C24" s="58" t="s">
         <v>34</v>
       </c>
-      <c r="B24" s="63"/>
-      <c r="C24" s="64" t="s">
+      <c r="D24" s="59"/>
+      <c r="E24" s="80"/>
+      <c r="F24" s="81"/>
+      <c r="G24" s="52"/>
+      <c r="H24" s="83"/>
+      <c r="I24" s="84"/>
+      <c r="K24" s="60">
+        <v>0.4</v>
+      </c>
+      <c r="L24" s="60">
+        <v>0.6</v>
+      </c>
+      <c r="M24" s="45"/>
+      <c r="Q24" s="13"/>
+    </row>
+    <row r="25" spans="1:25" ht="19.8">
+      <c r="A25" s="39" t="s">
         <v>35</v>
       </c>
-      <c r="D24" s="65"/>
-      <c r="E24" s="94"/>
-      <c r="F24" s="95"/>
-      <c r="G24" s="58"/>
-      <c r="H24" s="92"/>
-      <c r="I24" s="93"/>
-      <c r="K24" s="66">
-        <v>0.4</v>
-      </c>
-      <c r="L24" s="66">
-        <v>0.6</v>
-      </c>
-      <c r="M24" s="51" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q24" s="13"/>
-    </row>
-    <row r="25" spans="1:25" ht="19.8">
-      <c r="A25" s="45" t="s">
+      <c r="B25" s="40"/>
+      <c r="C25" s="41" t="s">
+        <v>29</v>
+      </c>
+      <c r="D25" s="61"/>
+      <c r="E25" s="76"/>
+      <c r="F25" s="77"/>
+      <c r="G25" s="52"/>
+      <c r="H25" s="80"/>
+      <c r="I25" s="81"/>
+      <c r="K25" s="44">
+        <v>0.5</v>
+      </c>
+      <c r="L25" s="44">
+        <v>2.4</v>
+      </c>
+      <c r="M25" s="45"/>
+      <c r="Q25" s="13"/>
+    </row>
+    <row r="26" spans="1:25" ht="19.8">
+      <c r="A26" s="62" t="s">
         <v>36</v>
       </c>
-      <c r="B25" s="46"/>
-      <c r="C25" s="47" t="s">
-        <v>30</v>
-      </c>
-      <c r="D25" s="67"/>
-      <c r="E25" s="101"/>
-      <c r="F25" s="102"/>
-      <c r="G25" s="58"/>
-      <c r="H25" s="94"/>
-      <c r="I25" s="95"/>
-      <c r="K25" s="50">
-        <v>0.5</v>
-      </c>
-      <c r="L25" s="50">
-        <v>2.4</v>
-      </c>
-      <c r="M25" s="51" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q25" s="13"/>
-    </row>
-    <row r="26" spans="1:25" ht="19.8">
-      <c r="A26" s="68" t="s">
+      <c r="B26" s="13"/>
+      <c r="C26" s="54" t="s">
         <v>37</v>
       </c>
-      <c r="B26" s="13"/>
-      <c r="C26" s="60" t="s">
+      <c r="D26" s="59"/>
+      <c r="E26" s="78"/>
+      <c r="F26" s="79"/>
+      <c r="G26" s="52"/>
+      <c r="H26" s="85"/>
+      <c r="I26" s="86"/>
+      <c r="K26" s="44">
+        <v>2289</v>
+      </c>
+      <c r="L26" s="44">
+        <v>2520</v>
+      </c>
+      <c r="M26" s="45"/>
+      <c r="N26" s="23"/>
+      <c r="Q26" s="13"/>
+      <c r="T26" s="49"/>
+    </row>
+    <row r="27" spans="1:25" ht="19.8">
+      <c r="A27" s="63" t="s">
         <v>38</v>
       </c>
-      <c r="D26" s="65"/>
-      <c r="E26" s="103"/>
-      <c r="F26" s="104"/>
-      <c r="G26" s="58"/>
-      <c r="H26" s="96"/>
-      <c r="I26" s="97"/>
-      <c r="K26" s="50">
-        <v>2289</v>
-      </c>
-      <c r="L26" s="50">
-        <v>2520</v>
-      </c>
-      <c r="M26" s="51" t="s">
-        <v>28</v>
-      </c>
-      <c r="N26" s="29"/>
-      <c r="Q26" s="13"/>
-      <c r="T26" s="55"/>
-    </row>
-    <row r="27" spans="1:25" ht="19.8">
-      <c r="A27" s="69" t="s">
+      <c r="B27" s="64"/>
+      <c r="C27" s="58" t="s">
+        <v>29</v>
+      </c>
+      <c r="D27" s="61"/>
+      <c r="E27" s="80"/>
+      <c r="F27" s="81"/>
+      <c r="G27" s="52"/>
+      <c r="H27" s="85"/>
+      <c r="I27" s="86"/>
+      <c r="K27" s="60">
+        <v>0.05</v>
+      </c>
+      <c r="L27" s="60">
+        <v>0.99</v>
+      </c>
+      <c r="M27" s="45"/>
+      <c r="N27" s="23"/>
+      <c r="Q27" s="13"/>
+      <c r="T27" s="46"/>
+    </row>
+    <row r="28" spans="1:25" ht="19.8">
+      <c r="A28" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="B27" s="70"/>
-      <c r="C27" s="64" t="s">
-        <v>30</v>
-      </c>
-      <c r="D27" s="67"/>
-      <c r="E27" s="94"/>
-      <c r="F27" s="95"/>
-      <c r="G27" s="58"/>
-      <c r="H27" s="96"/>
-      <c r="I27" s="97"/>
-      <c r="K27" s="66">
-        <v>0.05</v>
-      </c>
-      <c r="L27" s="66">
-        <v>0.99</v>
-      </c>
-      <c r="M27" s="51" t="s">
-        <v>28</v>
-      </c>
-      <c r="N27" s="29"/>
-      <c r="Q27" s="13"/>
-      <c r="T27" s="52"/>
-    </row>
-    <row r="28" spans="1:25" ht="19.8">
-      <c r="A28" s="45" t="s">
+      <c r="B28" s="40"/>
+      <c r="C28" s="41" t="s">
+        <v>29</v>
+      </c>
+      <c r="D28" s="65"/>
+      <c r="E28" s="80"/>
+      <c r="F28" s="81"/>
+      <c r="G28" s="52"/>
+      <c r="H28" s="85"/>
+      <c r="I28" s="86"/>
+      <c r="K28" s="44">
+        <v>2.5</v>
+      </c>
+      <c r="L28" s="44">
+        <v>4.5</v>
+      </c>
+      <c r="M28" s="45"/>
+      <c r="N28" s="23"/>
+      <c r="Y28" s="49"/>
+    </row>
+    <row r="29" spans="1:25" ht="19.8">
+      <c r="A29" s="39" t="s">
         <v>40</v>
       </c>
-      <c r="B28" s="46"/>
-      <c r="C28" s="47" t="s">
-        <v>30</v>
-      </c>
-      <c r="D28" s="71"/>
-      <c r="E28" s="94"/>
-      <c r="F28" s="95"/>
-      <c r="G28" s="58"/>
-      <c r="H28" s="96"/>
-      <c r="I28" s="97"/>
-      <c r="K28" s="50">
-        <v>2.5</v>
-      </c>
-      <c r="L28" s="50">
-        <v>4.5</v>
-      </c>
-      <c r="M28" s="51" t="s">
-        <v>28</v>
-      </c>
-      <c r="N28" s="29"/>
-      <c r="Y28" s="55"/>
-    </row>
-    <row r="29" spans="1:25" ht="19.8">
-      <c r="A29" s="45" t="s">
+      <c r="B29" s="40"/>
+      <c r="C29" s="41" t="s">
         <v>41</v>
       </c>
-      <c r="B29" s="46"/>
-      <c r="C29" s="47" t="s">
+      <c r="D29" s="65"/>
+      <c r="E29" s="80"/>
+      <c r="F29" s="81"/>
+      <c r="G29" s="52"/>
+      <c r="H29" s="85"/>
+      <c r="I29" s="86"/>
+      <c r="K29" s="44">
+        <v>3</v>
+      </c>
+      <c r="L29" s="44">
+        <v>12</v>
+      </c>
+      <c r="M29" s="45"/>
+      <c r="N29" s="23"/>
+      <c r="Y29" s="50"/>
+    </row>
+    <row r="30" spans="1:25" ht="25.5" customHeight="1">
+      <c r="A30" s="66" t="s">
         <v>42</v>
       </c>
-      <c r="D29" s="71"/>
-      <c r="E29" s="94"/>
-      <c r="F29" s="95"/>
-      <c r="G29" s="58"/>
-      <c r="H29" s="96"/>
-      <c r="I29" s="97"/>
-      <c r="K29" s="50">
-        <v>3</v>
-      </c>
-      <c r="L29" s="50">
-        <v>12</v>
-      </c>
-      <c r="M29" s="51" t="s">
-        <v>28</v>
-      </c>
-      <c r="N29" s="29"/>
-      <c r="Y29" s="56"/>
-    </row>
-    <row r="30" spans="1:25" ht="25.5" customHeight="1">
-      <c r="A30" s="72" t="s">
+      <c r="B30" s="82"/>
+      <c r="C30" s="82"/>
+      <c r="D30" s="82"/>
+      <c r="E30" s="82"/>
+      <c r="F30" s="82"/>
+      <c r="G30" s="82"/>
+      <c r="H30" s="67"/>
+      <c r="I30" s="67"/>
+      <c r="Y30" s="50"/>
+    </row>
+    <row r="31" spans="1:25" ht="25.5" customHeight="1">
+      <c r="A31" s="66"/>
+      <c r="B31" s="68"/>
+      <c r="C31" s="68"/>
+      <c r="D31" s="68"/>
+      <c r="E31" s="68"/>
+      <c r="F31" s="68"/>
+      <c r="G31" s="68"/>
+      <c r="H31" s="67"/>
+      <c r="I31" s="67"/>
+    </row>
+    <row r="32" spans="1:25" ht="19.8">
+      <c r="A32" s="69" t="s">
         <v>43</v>
       </c>
-      <c r="B30" s="91"/>
-      <c r="C30" s="91"/>
-      <c r="D30" s="91"/>
-      <c r="E30" s="91"/>
-      <c r="F30" s="91"/>
-      <c r="G30" s="91"/>
-      <c r="H30" s="73"/>
-      <c r="I30" s="73"/>
-      <c r="Y30" s="56"/>
-    </row>
-    <row r="31" spans="1:25" ht="25.5" customHeight="1">
-      <c r="A31" s="72"/>
-      <c r="B31" s="74"/>
-      <c r="C31" s="74"/>
-      <c r="D31" s="74"/>
-      <c r="E31" s="74"/>
-      <c r="F31" s="74"/>
-      <c r="G31" s="74"/>
-      <c r="H31" s="73"/>
-      <c r="I31" s="73"/>
-    </row>
-    <row r="32" spans="1:25" ht="19.8">
-      <c r="A32" s="75" t="s">
-        <v>44</v>
-      </c>
-      <c r="B32" s="76"/>
-      <c r="C32" s="76"/>
+      <c r="B32" s="70"/>
+      <c r="C32" s="70"/>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
@@ -1885,9 +1841,9 @@
       <c r="I32" s="1"/>
     </row>
     <row r="33" spans="1:9" ht="19.8">
-      <c r="A33" s="75"/>
-      <c r="B33" s="75"/>
-      <c r="C33" s="75"/>
+      <c r="A33" s="69"/>
+      <c r="B33" s="69"/>
+      <c r="C33" s="69"/>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
@@ -1896,16 +1852,16 @@
       <c r="I33" s="1"/>
     </row>
     <row r="34" spans="1:9" ht="17.399999999999999">
-      <c r="A34" s="77" t="s">
+      <c r="A34" s="71" t="s">
+        <v>44</v>
+      </c>
+      <c r="B34" s="71"/>
+      <c r="C34" s="71"/>
+      <c r="D34" s="71"/>
+      <c r="E34" s="71"/>
+      <c r="H34" s="72"/>
+      <c r="I34" s="72" t="s">
         <v>45</v>
-      </c>
-      <c r="B34" s="77"/>
-      <c r="C34" s="77"/>
-      <c r="D34" s="77"/>
-      <c r="E34" s="77"/>
-      <c r="H34" s="78"/>
-      <c r="I34" s="78" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="35" spans="1:9" ht="19.8">
@@ -1934,12 +1890,16 @@
   <protectedRanges>
     <protectedRange sqref="E10" name="Range1_3"/>
   </protectedRanges>
-  <mergeCells count="29">
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E29:F29"/>
+  <mergeCells count="30">
+    <mergeCell ref="E12:H13"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="Y17:Y19"/>
+    <mergeCell ref="A18:C19"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="E18:F19"/>
+    <mergeCell ref="G18:G19"/>
     <mergeCell ref="B30:G30"/>
     <mergeCell ref="H20:I20"/>
     <mergeCell ref="H21:I21"/>
@@ -1956,16 +1916,13 @@
     <mergeCell ref="E22:F22"/>
     <mergeCell ref="E23:F23"/>
     <mergeCell ref="E24:F24"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="Y17:Y19"/>
-    <mergeCell ref="A18:C19"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="E18:F19"/>
-    <mergeCell ref="G18:G19"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E29:F29"/>
   </mergeCells>
-  <conditionalFormatting sqref="E12:I16">
+  <conditionalFormatting sqref="I12:I16 E12 E14:H16">
     <cfRule type="cellIs" dxfId="1" priority="2" stopIfTrue="1" operator="equal">
       <formula>"NO PASSED"</formula>
     </cfRule>

</xml_diff>

<commit_message>
M3 QA Cord #503 - Implements Cord Test Data #93   - Update COA1, COA3
</commit_message>
<xml_diff>
--- a/05.Controls/M3.QA.Controls/Resources/Excels/COA1.xlsx
+++ b/05.Controls/M3.QA.Controls/Resources/Excels/COA1.xlsx
@@ -161,9 +161,6 @@
     <t>ELONG. AT 44 N</t>
   </si>
   <si>
-    <t>NUMBER OF TWISTS</t>
-  </si>
-  <si>
     <t xml:space="preserve">(t/10cm) </t>
   </si>
   <si>
@@ -173,12 +170,6 @@
     <t>(mm)</t>
   </si>
   <si>
-    <t xml:space="preserve">THERMAL SHRINKAGE </t>
-  </si>
-  <si>
-    <t>CORD SIZE</t>
-  </si>
-  <si>
     <t>(dtex)</t>
   </si>
   <si>
@@ -204,6 +195,15 @@
   </si>
   <si>
     <t>Retention  :  15  years</t>
+  </si>
+  <si>
+    <t>DENIER</t>
+  </si>
+  <si>
+    <t>SHRINKAGE</t>
+  </si>
+  <si>
+    <t>TWISTING NO</t>
   </si>
 </sst>
 </file>
@@ -756,6 +756,81 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="5" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="167" fontId="3" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -767,81 +842,6 @@
     </xf>
     <xf numFmtId="1" fontId="3" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="5" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="11">
@@ -910,7 +910,7 @@
         <xdr:cNvPr id="2" name="Picture 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{8C6984C9-0C37-400A-AFFE-0753047B13B4}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8C6984C9-0C37-400A-AFFE-0753047B13B4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1236,7 +1236,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1246,8 +1246,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Y36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12:H13"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.5546875" defaultRowHeight="13.2"/>
@@ -1431,10 +1431,10 @@
       <c r="B12" s="19"/>
       <c r="C12" s="13"/>
       <c r="D12" s="13"/>
-      <c r="E12" s="99"/>
-      <c r="F12" s="100"/>
-      <c r="G12" s="100"/>
-      <c r="H12" s="101"/>
+      <c r="E12" s="76"/>
+      <c r="F12" s="77"/>
+      <c r="G12" s="77"/>
+      <c r="H12" s="78"/>
       <c r="I12" s="20"/>
       <c r="N12" s="74"/>
     </row>
@@ -1445,10 +1445,10 @@
       <c r="B13" s="21"/>
       <c r="C13" s="22"/>
       <c r="D13" s="13"/>
-      <c r="E13" s="102"/>
-      <c r="F13" s="103"/>
-      <c r="G13" s="103"/>
-      <c r="H13" s="104"/>
+      <c r="E13" s="79"/>
+      <c r="F13" s="80"/>
+      <c r="G13" s="80"/>
+      <c r="H13" s="81"/>
       <c r="I13" s="20"/>
       <c r="K13" s="23"/>
       <c r="N13" s="74"/>
@@ -1460,14 +1460,14 @@
       <c r="B14" s="24"/>
       <c r="C14" s="13"/>
       <c r="D14" s="13"/>
-      <c r="E14" s="87" t="s">
+      <c r="E14" s="82" t="s">
         <v>13</v>
       </c>
-      <c r="F14" s="88"/>
-      <c r="G14" s="87" t="s">
+      <c r="F14" s="83"/>
+      <c r="G14" s="82" t="s">
         <v>14</v>
       </c>
-      <c r="H14" s="88"/>
+      <c r="H14" s="83"/>
       <c r="I14" s="25" t="s">
         <v>15</v>
       </c>
@@ -1477,8 +1477,8 @@
       <c r="A15" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="89"/>
-      <c r="C15" s="89"/>
+      <c r="B15" s="84"/>
+      <c r="C15" s="84"/>
       <c r="D15" s="13"/>
       <c r="E15" s="26"/>
       <c r="F15" s="27"/>
@@ -1516,22 +1516,22 @@
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
       <c r="N17" s="74"/>
-      <c r="Y17" s="90"/>
+      <c r="Y17" s="85"/>
     </row>
     <row r="18" spans="1:25" ht="19.8">
-      <c r="A18" s="91" t="s">
+      <c r="A18" s="86" t="s">
         <v>20</v>
       </c>
-      <c r="B18" s="92"/>
-      <c r="C18" s="93"/>
-      <c r="D18" s="97" t="s">
+      <c r="B18" s="87"/>
+      <c r="C18" s="88"/>
+      <c r="D18" s="92" t="s">
         <v>21</v>
       </c>
-      <c r="E18" s="91" t="s">
+      <c r="E18" s="86" t="s">
         <v>22</v>
       </c>
-      <c r="F18" s="93"/>
-      <c r="G18" s="97" t="s">
+      <c r="F18" s="88"/>
+      <c r="G18" s="92" t="s">
         <v>23</v>
       </c>
       <c r="H18" s="34" t="s">
@@ -1541,16 +1541,16 @@
       <c r="N18" s="74"/>
       <c r="Q18" s="13"/>
       <c r="T18" s="36"/>
-      <c r="Y18" s="90"/>
+      <c r="Y18" s="85"/>
     </row>
     <row r="19" spans="1:25" ht="21.6">
-      <c r="A19" s="94"/>
-      <c r="B19" s="95"/>
-      <c r="C19" s="96"/>
-      <c r="D19" s="98"/>
-      <c r="E19" s="94"/>
-      <c r="F19" s="96"/>
-      <c r="G19" s="98"/>
+      <c r="A19" s="89"/>
+      <c r="B19" s="90"/>
+      <c r="C19" s="91"/>
+      <c r="D19" s="93"/>
+      <c r="E19" s="89"/>
+      <c r="F19" s="91"/>
+      <c r="G19" s="93"/>
       <c r="H19" s="37" t="s">
         <v>25</v>
       </c>
@@ -1560,7 +1560,7 @@
       <c r="M19" s="23"/>
       <c r="Q19" s="13"/>
       <c r="T19" s="36"/>
-      <c r="Y19" s="90"/>
+      <c r="Y19" s="85"/>
     </row>
     <row r="20" spans="1:25" ht="19.8">
       <c r="A20" s="39" t="s">
@@ -1571,11 +1571,11 @@
         <v>27</v>
       </c>
       <c r="D20" s="42"/>
-      <c r="E20" s="76"/>
-      <c r="F20" s="77"/>
+      <c r="E20" s="101"/>
+      <c r="F20" s="102"/>
       <c r="G20" s="43"/>
-      <c r="H20" s="83"/>
-      <c r="I20" s="84"/>
+      <c r="H20" s="95"/>
+      <c r="I20" s="96"/>
       <c r="K20" s="44">
         <v>136</v>
       </c>
@@ -1595,11 +1595,11 @@
         <v>29</v>
       </c>
       <c r="D21" s="48"/>
-      <c r="E21" s="76"/>
-      <c r="F21" s="77"/>
+      <c r="E21" s="101"/>
+      <c r="F21" s="102"/>
       <c r="G21" s="43"/>
-      <c r="H21" s="83"/>
-      <c r="I21" s="84"/>
+      <c r="H21" s="95"/>
+      <c r="I21" s="96"/>
       <c r="K21" s="44">
         <v>11</v>
       </c>
@@ -1620,11 +1620,11 @@
         <v>29</v>
       </c>
       <c r="D22" s="51"/>
-      <c r="E22" s="76"/>
-      <c r="F22" s="77"/>
+      <c r="E22" s="101"/>
+      <c r="F22" s="102"/>
       <c r="G22" s="52"/>
-      <c r="H22" s="83"/>
-      <c r="I22" s="84"/>
+      <c r="H22" s="95"/>
+      <c r="I22" s="96"/>
       <c r="K22" s="44">
         <v>1.99</v>
       </c>
@@ -1637,18 +1637,18 @@
     </row>
     <row r="23" spans="1:25" ht="24.75" customHeight="1">
       <c r="A23" s="53" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="54" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D23" s="55"/>
-      <c r="E23" s="76"/>
-      <c r="F23" s="77"/>
+      <c r="E23" s="101"/>
+      <c r="F23" s="102"/>
       <c r="G23" s="52"/>
-      <c r="H23" s="83"/>
-      <c r="I23" s="84"/>
+      <c r="H23" s="95"/>
+      <c r="I23" s="96"/>
       <c r="K23" s="44">
         <v>10.49</v>
       </c>
@@ -1660,18 +1660,18 @@
     </row>
     <row r="24" spans="1:25" ht="19.8">
       <c r="A24" s="56" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B24" s="57"/>
       <c r="C24" s="58" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D24" s="59"/>
-      <c r="E24" s="80"/>
-      <c r="F24" s="81"/>
+      <c r="E24" s="97"/>
+      <c r="F24" s="98"/>
       <c r="G24" s="52"/>
-      <c r="H24" s="83"/>
-      <c r="I24" s="84"/>
+      <c r="H24" s="95"/>
+      <c r="I24" s="96"/>
       <c r="K24" s="60">
         <v>0.4</v>
       </c>
@@ -1683,18 +1683,18 @@
     </row>
     <row r="25" spans="1:25" ht="19.8">
       <c r="A25" s="39" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="B25" s="40"/>
       <c r="C25" s="41" t="s">
         <v>29</v>
       </c>
       <c r="D25" s="61"/>
-      <c r="E25" s="76"/>
-      <c r="F25" s="77"/>
+      <c r="E25" s="101"/>
+      <c r="F25" s="102"/>
       <c r="G25" s="52"/>
-      <c r="H25" s="80"/>
-      <c r="I25" s="81"/>
+      <c r="H25" s="97"/>
+      <c r="I25" s="98"/>
       <c r="K25" s="44">
         <v>0.5</v>
       </c>
@@ -1706,18 +1706,18 @@
     </row>
     <row r="26" spans="1:25" ht="19.8">
       <c r="A26" s="62" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="B26" s="13"/>
       <c r="C26" s="54" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D26" s="59"/>
-      <c r="E26" s="78"/>
-      <c r="F26" s="79"/>
+      <c r="E26" s="103"/>
+      <c r="F26" s="104"/>
       <c r="G26" s="52"/>
-      <c r="H26" s="85"/>
-      <c r="I26" s="86"/>
+      <c r="H26" s="99"/>
+      <c r="I26" s="100"/>
       <c r="K26" s="44">
         <v>2289</v>
       </c>
@@ -1731,18 +1731,18 @@
     </row>
     <row r="27" spans="1:25" ht="19.8">
       <c r="A27" s="63" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B27" s="64"/>
       <c r="C27" s="58" t="s">
         <v>29</v>
       </c>
       <c r="D27" s="61"/>
-      <c r="E27" s="80"/>
-      <c r="F27" s="81"/>
+      <c r="E27" s="97"/>
+      <c r="F27" s="98"/>
       <c r="G27" s="52"/>
-      <c r="H27" s="85"/>
-      <c r="I27" s="86"/>
+      <c r="H27" s="99"/>
+      <c r="I27" s="100"/>
       <c r="K27" s="60">
         <v>0.05</v>
       </c>
@@ -1756,18 +1756,18 @@
     </row>
     <row r="28" spans="1:25" ht="19.8">
       <c r="A28" s="39" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B28" s="40"/>
       <c r="C28" s="41" t="s">
         <v>29</v>
       </c>
       <c r="D28" s="65"/>
-      <c r="E28" s="80"/>
-      <c r="F28" s="81"/>
+      <c r="E28" s="97"/>
+      <c r="F28" s="98"/>
       <c r="G28" s="52"/>
-      <c r="H28" s="85"/>
-      <c r="I28" s="86"/>
+      <c r="H28" s="99"/>
+      <c r="I28" s="100"/>
       <c r="K28" s="44">
         <v>2.5</v>
       </c>
@@ -1780,18 +1780,18 @@
     </row>
     <row r="29" spans="1:25" ht="19.8">
       <c r="A29" s="39" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B29" s="40"/>
       <c r="C29" s="41" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D29" s="65"/>
-      <c r="E29" s="80"/>
-      <c r="F29" s="81"/>
+      <c r="E29" s="97"/>
+      <c r="F29" s="98"/>
       <c r="G29" s="52"/>
-      <c r="H29" s="85"/>
-      <c r="I29" s="86"/>
+      <c r="H29" s="99"/>
+      <c r="I29" s="100"/>
       <c r="K29" s="44">
         <v>3</v>
       </c>
@@ -1804,14 +1804,14 @@
     </row>
     <row r="30" spans="1:25" ht="25.5" customHeight="1">
       <c r="A30" s="66" t="s">
-        <v>42</v>
-      </c>
-      <c r="B30" s="82"/>
-      <c r="C30" s="82"/>
-      <c r="D30" s="82"/>
-      <c r="E30" s="82"/>
-      <c r="F30" s="82"/>
-      <c r="G30" s="82"/>
+        <v>39</v>
+      </c>
+      <c r="B30" s="94"/>
+      <c r="C30" s="94"/>
+      <c r="D30" s="94"/>
+      <c r="E30" s="94"/>
+      <c r="F30" s="94"/>
+      <c r="G30" s="94"/>
       <c r="H30" s="67"/>
       <c r="I30" s="67"/>
       <c r="Y30" s="50"/>
@@ -1829,7 +1829,7 @@
     </row>
     <row r="32" spans="1:25" ht="19.8">
       <c r="A32" s="69" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B32" s="70"/>
       <c r="C32" s="70"/>
@@ -1853,7 +1853,7 @@
     </row>
     <row r="34" spans="1:9" ht="17.399999999999999">
       <c r="A34" s="71" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B34" s="71"/>
       <c r="C34" s="71"/>
@@ -1861,7 +1861,7 @@
       <c r="E34" s="71"/>
       <c r="H34" s="72"/>
       <c r="I34" s="72" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="35" spans="1:9" ht="19.8">
@@ -1891,15 +1891,11 @@
     <protectedRange sqref="E10" name="Range1_3"/>
   </protectedRanges>
   <mergeCells count="30">
-    <mergeCell ref="E12:H13"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="Y17:Y19"/>
-    <mergeCell ref="A18:C19"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="E18:F19"/>
-    <mergeCell ref="G18:G19"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E29:F29"/>
     <mergeCell ref="B30:G30"/>
     <mergeCell ref="H20:I20"/>
     <mergeCell ref="H21:I21"/>
@@ -1916,11 +1912,15 @@
     <mergeCell ref="E22:F22"/>
     <mergeCell ref="E23:F23"/>
     <mergeCell ref="E24:F24"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="E12:H13"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="Y17:Y19"/>
+    <mergeCell ref="A18:C19"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="E18:F19"/>
+    <mergeCell ref="G18:G19"/>
   </mergeCells>
   <conditionalFormatting sqref="I12:I16 E12 E14:H16">
     <cfRule type="cellIs" dxfId="1" priority="2" stopIfTrue="1" operator="equal">

</xml_diff>

<commit_message>
M3 QA Cord #520 - Update excel export   - Change font size in excel files
</commit_message>
<xml_diff>
--- a/05.Controls/M3.QA.Controls/Resources/Excels/COA1.xlsx
+++ b/05.Controls/M3.QA.Controls/Resources/Excels/COA1.xlsx
@@ -350,10 +350,10 @@
       <family val="1"/>
     </font>
     <font>
-      <sz val="18"/>
-      <name val="AngsanaUPC"/>
+      <b/>
+      <sz val="50"/>
+      <name val="Angsana New"/>
       <family val="1"/>
-      <charset val="222"/>
     </font>
   </fonts>
   <fills count="2">
@@ -756,23 +756,38 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -810,38 +825,23 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="11">
@@ -910,7 +910,7 @@
         <xdr:cNvPr id="2" name="Picture 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8C6984C9-0C37-400A-AFFE-0753047B13B4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{8C6984C9-0C37-400A-AFFE-0753047B13B4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1236,7 +1236,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1246,8 +1246,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Y36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.5546875" defaultRowHeight="13.2"/>
@@ -1255,7 +1255,7 @@
     <col min="1" max="1" width="10.77734375" style="2" customWidth="1"/>
     <col min="2" max="2" width="8.77734375" style="2" customWidth="1"/>
     <col min="3" max="7" width="8.109375" style="2" customWidth="1"/>
-    <col min="8" max="8" width="7.21875" style="2" customWidth="1"/>
+    <col min="8" max="8" width="11.5546875" style="2" customWidth="1"/>
     <col min="9" max="9" width="12" style="2" customWidth="1"/>
     <col min="10" max="13" width="7.5546875" style="2"/>
     <col min="14" max="14" width="10.44140625" style="2" customWidth="1"/>
@@ -1431,10 +1431,10 @@
       <c r="B12" s="19"/>
       <c r="C12" s="13"/>
       <c r="D12" s="13"/>
-      <c r="E12" s="76"/>
-      <c r="F12" s="77"/>
-      <c r="G12" s="77"/>
-      <c r="H12" s="78"/>
+      <c r="E12" s="99"/>
+      <c r="F12" s="100"/>
+      <c r="G12" s="100"/>
+      <c r="H12" s="101"/>
       <c r="I12" s="20"/>
       <c r="N12" s="74"/>
     </row>
@@ -1445,10 +1445,10 @@
       <c r="B13" s="21"/>
       <c r="C13" s="22"/>
       <c r="D13" s="13"/>
-      <c r="E13" s="79"/>
-      <c r="F13" s="80"/>
-      <c r="G13" s="80"/>
-      <c r="H13" s="81"/>
+      <c r="E13" s="102"/>
+      <c r="F13" s="103"/>
+      <c r="G13" s="103"/>
+      <c r="H13" s="104"/>
       <c r="I13" s="20"/>
       <c r="K13" s="23"/>
       <c r="N13" s="74"/>
@@ -1460,14 +1460,14 @@
       <c r="B14" s="24"/>
       <c r="C14" s="13"/>
       <c r="D14" s="13"/>
-      <c r="E14" s="82" t="s">
+      <c r="E14" s="87" t="s">
         <v>13</v>
       </c>
-      <c r="F14" s="83"/>
-      <c r="G14" s="82" t="s">
+      <c r="F14" s="88"/>
+      <c r="G14" s="87" t="s">
         <v>14</v>
       </c>
-      <c r="H14" s="83"/>
+      <c r="H14" s="88"/>
       <c r="I14" s="25" t="s">
         <v>15</v>
       </c>
@@ -1477,8 +1477,8 @@
       <c r="A15" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="84"/>
-      <c r="C15" s="84"/>
+      <c r="B15" s="89"/>
+      <c r="C15" s="89"/>
       <c r="D15" s="13"/>
       <c r="E15" s="26"/>
       <c r="F15" s="27"/>
@@ -1516,22 +1516,22 @@
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
       <c r="N17" s="74"/>
-      <c r="Y17" s="85"/>
+      <c r="Y17" s="90"/>
     </row>
     <row r="18" spans="1:25" ht="19.8">
-      <c r="A18" s="86" t="s">
+      <c r="A18" s="91" t="s">
         <v>20</v>
       </c>
-      <c r="B18" s="87"/>
-      <c r="C18" s="88"/>
-      <c r="D18" s="92" t="s">
+      <c r="B18" s="92"/>
+      <c r="C18" s="93"/>
+      <c r="D18" s="97" t="s">
         <v>21</v>
       </c>
-      <c r="E18" s="86" t="s">
+      <c r="E18" s="91" t="s">
         <v>22</v>
       </c>
-      <c r="F18" s="88"/>
-      <c r="G18" s="92" t="s">
+      <c r="F18" s="93"/>
+      <c r="G18" s="97" t="s">
         <v>23</v>
       </c>
       <c r="H18" s="34" t="s">
@@ -1541,16 +1541,16 @@
       <c r="N18" s="74"/>
       <c r="Q18" s="13"/>
       <c r="T18" s="36"/>
-      <c r="Y18" s="85"/>
+      <c r="Y18" s="90"/>
     </row>
     <row r="19" spans="1:25" ht="21.6">
-      <c r="A19" s="89"/>
-      <c r="B19" s="90"/>
-      <c r="C19" s="91"/>
-      <c r="D19" s="93"/>
-      <c r="E19" s="89"/>
-      <c r="F19" s="91"/>
-      <c r="G19" s="93"/>
+      <c r="A19" s="94"/>
+      <c r="B19" s="95"/>
+      <c r="C19" s="96"/>
+      <c r="D19" s="98"/>
+      <c r="E19" s="94"/>
+      <c r="F19" s="96"/>
+      <c r="G19" s="98"/>
       <c r="H19" s="37" t="s">
         <v>25</v>
       </c>
@@ -1560,7 +1560,7 @@
       <c r="M19" s="23"/>
       <c r="Q19" s="13"/>
       <c r="T19" s="36"/>
-      <c r="Y19" s="85"/>
+      <c r="Y19" s="90"/>
     </row>
     <row r="20" spans="1:25" ht="19.8">
       <c r="A20" s="39" t="s">
@@ -1571,11 +1571,11 @@
         <v>27</v>
       </c>
       <c r="D20" s="42"/>
-      <c r="E20" s="101"/>
-      <c r="F20" s="102"/>
+      <c r="E20" s="76"/>
+      <c r="F20" s="77"/>
       <c r="G20" s="43"/>
-      <c r="H20" s="95"/>
-      <c r="I20" s="96"/>
+      <c r="H20" s="83"/>
+      <c r="I20" s="84"/>
       <c r="K20" s="44">
         <v>136</v>
       </c>
@@ -1595,11 +1595,11 @@
         <v>29</v>
       </c>
       <c r="D21" s="48"/>
-      <c r="E21" s="101"/>
-      <c r="F21" s="102"/>
+      <c r="E21" s="76"/>
+      <c r="F21" s="77"/>
       <c r="G21" s="43"/>
-      <c r="H21" s="95"/>
-      <c r="I21" s="96"/>
+      <c r="H21" s="83"/>
+      <c r="I21" s="84"/>
       <c r="K21" s="44">
         <v>11</v>
       </c>
@@ -1620,11 +1620,11 @@
         <v>29</v>
       </c>
       <c r="D22" s="51"/>
-      <c r="E22" s="101"/>
-      <c r="F22" s="102"/>
+      <c r="E22" s="76"/>
+      <c r="F22" s="77"/>
       <c r="G22" s="52"/>
-      <c r="H22" s="95"/>
-      <c r="I22" s="96"/>
+      <c r="H22" s="83"/>
+      <c r="I22" s="84"/>
       <c r="K22" s="44">
         <v>1.99</v>
       </c>
@@ -1644,11 +1644,11 @@
         <v>31</v>
       </c>
       <c r="D23" s="55"/>
-      <c r="E23" s="101"/>
-      <c r="F23" s="102"/>
+      <c r="E23" s="76"/>
+      <c r="F23" s="77"/>
       <c r="G23" s="52"/>
-      <c r="H23" s="95"/>
-      <c r="I23" s="96"/>
+      <c r="H23" s="83"/>
+      <c r="I23" s="84"/>
       <c r="K23" s="44">
         <v>10.49</v>
       </c>
@@ -1667,11 +1667,11 @@
         <v>33</v>
       </c>
       <c r="D24" s="59"/>
-      <c r="E24" s="97"/>
-      <c r="F24" s="98"/>
+      <c r="E24" s="80"/>
+      <c r="F24" s="81"/>
       <c r="G24" s="52"/>
-      <c r="H24" s="95"/>
-      <c r="I24" s="96"/>
+      <c r="H24" s="83"/>
+      <c r="I24" s="84"/>
       <c r="K24" s="60">
         <v>0.4</v>
       </c>
@@ -1690,11 +1690,11 @@
         <v>29</v>
       </c>
       <c r="D25" s="61"/>
-      <c r="E25" s="101"/>
-      <c r="F25" s="102"/>
+      <c r="E25" s="76"/>
+      <c r="F25" s="77"/>
       <c r="G25" s="52"/>
-      <c r="H25" s="97"/>
-      <c r="I25" s="98"/>
+      <c r="H25" s="80"/>
+      <c r="I25" s="81"/>
       <c r="K25" s="44">
         <v>0.5</v>
       </c>
@@ -1713,11 +1713,11 @@
         <v>34</v>
       </c>
       <c r="D26" s="59"/>
-      <c r="E26" s="103"/>
-      <c r="F26" s="104"/>
+      <c r="E26" s="78"/>
+      <c r="F26" s="79"/>
       <c r="G26" s="52"/>
-      <c r="H26" s="99"/>
-      <c r="I26" s="100"/>
+      <c r="H26" s="85"/>
+      <c r="I26" s="86"/>
       <c r="K26" s="44">
         <v>2289</v>
       </c>
@@ -1738,11 +1738,11 @@
         <v>29</v>
       </c>
       <c r="D27" s="61"/>
-      <c r="E27" s="97"/>
-      <c r="F27" s="98"/>
+      <c r="E27" s="80"/>
+      <c r="F27" s="81"/>
       <c r="G27" s="52"/>
-      <c r="H27" s="99"/>
-      <c r="I27" s="100"/>
+      <c r="H27" s="85"/>
+      <c r="I27" s="86"/>
       <c r="K27" s="60">
         <v>0.05</v>
       </c>
@@ -1763,11 +1763,11 @@
         <v>29</v>
       </c>
       <c r="D28" s="65"/>
-      <c r="E28" s="97"/>
-      <c r="F28" s="98"/>
+      <c r="E28" s="80"/>
+      <c r="F28" s="81"/>
       <c r="G28" s="52"/>
-      <c r="H28" s="99"/>
-      <c r="I28" s="100"/>
+      <c r="H28" s="85"/>
+      <c r="I28" s="86"/>
       <c r="K28" s="44">
         <v>2.5</v>
       </c>
@@ -1787,11 +1787,11 @@
         <v>38</v>
       </c>
       <c r="D29" s="65"/>
-      <c r="E29" s="97"/>
-      <c r="F29" s="98"/>
+      <c r="E29" s="80"/>
+      <c r="F29" s="81"/>
       <c r="G29" s="52"/>
-      <c r="H29" s="99"/>
-      <c r="I29" s="100"/>
+      <c r="H29" s="85"/>
+      <c r="I29" s="86"/>
       <c r="K29" s="44">
         <v>3</v>
       </c>
@@ -1806,12 +1806,12 @@
       <c r="A30" s="66" t="s">
         <v>39</v>
       </c>
-      <c r="B30" s="94"/>
-      <c r="C30" s="94"/>
-      <c r="D30" s="94"/>
-      <c r="E30" s="94"/>
-      <c r="F30" s="94"/>
-      <c r="G30" s="94"/>
+      <c r="B30" s="82"/>
+      <c r="C30" s="82"/>
+      <c r="D30" s="82"/>
+      <c r="E30" s="82"/>
+      <c r="F30" s="82"/>
+      <c r="G30" s="82"/>
       <c r="H30" s="67"/>
       <c r="I30" s="67"/>
       <c r="Y30" s="50"/>
@@ -1891,11 +1891,15 @@
     <protectedRange sqref="E10" name="Range1_3"/>
   </protectedRanges>
   <mergeCells count="30">
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="E12:H13"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="Y17:Y19"/>
+    <mergeCell ref="A18:C19"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="E18:F19"/>
+    <mergeCell ref="G18:G19"/>
     <mergeCell ref="B30:G30"/>
     <mergeCell ref="H20:I20"/>
     <mergeCell ref="H21:I21"/>
@@ -1912,15 +1916,11 @@
     <mergeCell ref="E22:F22"/>
     <mergeCell ref="E23:F23"/>
     <mergeCell ref="E24:F24"/>
-    <mergeCell ref="E12:H13"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="Y17:Y19"/>
-    <mergeCell ref="A18:C19"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="E18:F19"/>
-    <mergeCell ref="G18:G19"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E29:F29"/>
   </mergeCells>
   <conditionalFormatting sqref="I12:I16 E12 E14:H16">
     <cfRule type="cellIs" dxfId="1" priority="2" stopIfTrue="1" operator="equal">

</xml_diff>

<commit_message>
M3 QA Cord #521 - Update excel export   - COA 1, 2, 3
</commit_message>
<xml_diff>
--- a/05.Controls/M3.QA.Controls/Resources/Excels/COA1.xlsx
+++ b/05.Controls/M3.QA.Controls/Resources/Excels/COA1.xlsx
@@ -756,6 +756,81 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="5" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="167" fontId="3" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -767,81 +842,6 @@
     </xf>
     <xf numFmtId="1" fontId="3" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="5" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="11">
@@ -910,7 +910,7 @@
         <xdr:cNvPr id="2" name="Picture 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{8C6984C9-0C37-400A-AFFE-0753047B13B4}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8C6984C9-0C37-400A-AFFE-0753047B13B4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1236,7 +1236,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1247,7 +1247,7 @@
   <dimension ref="A1:Y36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.5546875" defaultRowHeight="13.2"/>
@@ -1431,10 +1431,10 @@
       <c r="B12" s="19"/>
       <c r="C12" s="13"/>
       <c r="D12" s="13"/>
-      <c r="E12" s="99"/>
-      <c r="F12" s="100"/>
-      <c r="G12" s="100"/>
-      <c r="H12" s="101"/>
+      <c r="E12" s="76"/>
+      <c r="F12" s="77"/>
+      <c r="G12" s="77"/>
+      <c r="H12" s="78"/>
       <c r="I12" s="20"/>
       <c r="N12" s="74"/>
     </row>
@@ -1445,10 +1445,10 @@
       <c r="B13" s="21"/>
       <c r="C13" s="22"/>
       <c r="D13" s="13"/>
-      <c r="E13" s="102"/>
-      <c r="F13" s="103"/>
-      <c r="G13" s="103"/>
-      <c r="H13" s="104"/>
+      <c r="E13" s="79"/>
+      <c r="F13" s="80"/>
+      <c r="G13" s="80"/>
+      <c r="H13" s="81"/>
       <c r="I13" s="20"/>
       <c r="K13" s="23"/>
       <c r="N13" s="74"/>
@@ -1460,14 +1460,14 @@
       <c r="B14" s="24"/>
       <c r="C14" s="13"/>
       <c r="D14" s="13"/>
-      <c r="E14" s="87" t="s">
+      <c r="E14" s="82" t="s">
         <v>13</v>
       </c>
-      <c r="F14" s="88"/>
-      <c r="G14" s="87" t="s">
+      <c r="F14" s="83"/>
+      <c r="G14" s="82" t="s">
         <v>14</v>
       </c>
-      <c r="H14" s="88"/>
+      <c r="H14" s="83"/>
       <c r="I14" s="25" t="s">
         <v>15</v>
       </c>
@@ -1477,8 +1477,8 @@
       <c r="A15" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="89"/>
-      <c r="C15" s="89"/>
+      <c r="B15" s="84"/>
+      <c r="C15" s="84"/>
       <c r="D15" s="13"/>
       <c r="E15" s="26"/>
       <c r="F15" s="27"/>
@@ -1516,22 +1516,22 @@
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
       <c r="N17" s="74"/>
-      <c r="Y17" s="90"/>
+      <c r="Y17" s="85"/>
     </row>
     <row r="18" spans="1:25" ht="19.8">
-      <c r="A18" s="91" t="s">
+      <c r="A18" s="86" t="s">
         <v>20</v>
       </c>
-      <c r="B18" s="92"/>
-      <c r="C18" s="93"/>
-      <c r="D18" s="97" t="s">
+      <c r="B18" s="87"/>
+      <c r="C18" s="88"/>
+      <c r="D18" s="92" t="s">
         <v>21</v>
       </c>
-      <c r="E18" s="91" t="s">
+      <c r="E18" s="86" t="s">
         <v>22</v>
       </c>
-      <c r="F18" s="93"/>
-      <c r="G18" s="97" t="s">
+      <c r="F18" s="88"/>
+      <c r="G18" s="92" t="s">
         <v>23</v>
       </c>
       <c r="H18" s="34" t="s">
@@ -1541,16 +1541,16 @@
       <c r="N18" s="74"/>
       <c r="Q18" s="13"/>
       <c r="T18" s="36"/>
-      <c r="Y18" s="90"/>
+      <c r="Y18" s="85"/>
     </row>
     <row r="19" spans="1:25" ht="21.6">
-      <c r="A19" s="94"/>
-      <c r="B19" s="95"/>
-      <c r="C19" s="96"/>
-      <c r="D19" s="98"/>
-      <c r="E19" s="94"/>
-      <c r="F19" s="96"/>
-      <c r="G19" s="98"/>
+      <c r="A19" s="89"/>
+      <c r="B19" s="90"/>
+      <c r="C19" s="91"/>
+      <c r="D19" s="93"/>
+      <c r="E19" s="89"/>
+      <c r="F19" s="91"/>
+      <c r="G19" s="93"/>
       <c r="H19" s="37" t="s">
         <v>25</v>
       </c>
@@ -1560,7 +1560,7 @@
       <c r="M19" s="23"/>
       <c r="Q19" s="13"/>
       <c r="T19" s="36"/>
-      <c r="Y19" s="90"/>
+      <c r="Y19" s="85"/>
     </row>
     <row r="20" spans="1:25" ht="19.8">
       <c r="A20" s="39" t="s">
@@ -1571,17 +1571,13 @@
         <v>27</v>
       </c>
       <c r="D20" s="42"/>
-      <c r="E20" s="76"/>
-      <c r="F20" s="77"/>
+      <c r="E20" s="101"/>
+      <c r="F20" s="102"/>
       <c r="G20" s="43"/>
-      <c r="H20" s="83"/>
-      <c r="I20" s="84"/>
-      <c r="K20" s="44">
-        <v>136</v>
-      </c>
-      <c r="L20" s="44">
-        <v>180</v>
-      </c>
+      <c r="H20" s="95"/>
+      <c r="I20" s="96"/>
+      <c r="K20" s="44"/>
+      <c r="L20" s="44"/>
       <c r="M20" s="45"/>
       <c r="Q20" s="13"/>
       <c r="T20" s="46"/>
@@ -1595,17 +1591,13 @@
         <v>29</v>
       </c>
       <c r="D21" s="48"/>
-      <c r="E21" s="76"/>
-      <c r="F21" s="77"/>
+      <c r="E21" s="101"/>
+      <c r="F21" s="102"/>
       <c r="G21" s="43"/>
-      <c r="H21" s="83"/>
-      <c r="I21" s="84"/>
-      <c r="K21" s="44">
-        <v>11</v>
-      </c>
-      <c r="L21" s="44">
-        <v>18</v>
-      </c>
+      <c r="H21" s="95"/>
+      <c r="I21" s="96"/>
+      <c r="K21" s="44"/>
+      <c r="L21" s="44"/>
       <c r="M21" s="45"/>
       <c r="Q21" s="1"/>
       <c r="T21" s="49"/>
@@ -1620,17 +1612,13 @@
         <v>29</v>
       </c>
       <c r="D22" s="51"/>
-      <c r="E22" s="76"/>
-      <c r="F22" s="77"/>
+      <c r="E22" s="101"/>
+      <c r="F22" s="102"/>
       <c r="G22" s="52"/>
-      <c r="H22" s="83"/>
-      <c r="I22" s="84"/>
-      <c r="K22" s="44">
-        <v>1.99</v>
-      </c>
-      <c r="L22" s="44">
-        <v>4.99</v>
-      </c>
+      <c r="H22" s="95"/>
+      <c r="I22" s="96"/>
+      <c r="K22" s="44"/>
+      <c r="L22" s="44"/>
       <c r="M22" s="45"/>
       <c r="Q22" s="1"/>
       <c r="Y22" s="49"/>
@@ -1644,17 +1632,13 @@
         <v>31</v>
       </c>
       <c r="D23" s="55"/>
-      <c r="E23" s="76"/>
-      <c r="F23" s="77"/>
+      <c r="E23" s="101"/>
+      <c r="F23" s="102"/>
       <c r="G23" s="52"/>
-      <c r="H23" s="83"/>
-      <c r="I23" s="84"/>
-      <c r="K23" s="44">
-        <v>10.49</v>
-      </c>
-      <c r="L23" s="44">
-        <v>12.49</v>
-      </c>
+      <c r="H23" s="95"/>
+      <c r="I23" s="96"/>
+      <c r="K23" s="44"/>
+      <c r="L23" s="44"/>
       <c r="M23" s="45"/>
       <c r="Q23" s="13"/>
     </row>
@@ -1667,17 +1651,13 @@
         <v>33</v>
       </c>
       <c r="D24" s="59"/>
-      <c r="E24" s="80"/>
-      <c r="F24" s="81"/>
+      <c r="E24" s="97"/>
+      <c r="F24" s="98"/>
       <c r="G24" s="52"/>
-      <c r="H24" s="83"/>
-      <c r="I24" s="84"/>
-      <c r="K24" s="60">
-        <v>0.4</v>
-      </c>
-      <c r="L24" s="60">
-        <v>0.6</v>
-      </c>
+      <c r="H24" s="95"/>
+      <c r="I24" s="96"/>
+      <c r="K24" s="60"/>
+      <c r="L24" s="60"/>
       <c r="M24" s="45"/>
       <c r="Q24" s="13"/>
     </row>
@@ -1690,17 +1670,13 @@
         <v>29</v>
       </c>
       <c r="D25" s="61"/>
-      <c r="E25" s="76"/>
-      <c r="F25" s="77"/>
+      <c r="E25" s="101"/>
+      <c r="F25" s="102"/>
       <c r="G25" s="52"/>
-      <c r="H25" s="80"/>
-      <c r="I25" s="81"/>
-      <c r="K25" s="44">
-        <v>0.5</v>
-      </c>
-      <c r="L25" s="44">
-        <v>2.4</v>
-      </c>
+      <c r="H25" s="97"/>
+      <c r="I25" s="98"/>
+      <c r="K25" s="44"/>
+      <c r="L25" s="44"/>
       <c r="M25" s="45"/>
       <c r="Q25" s="13"/>
     </row>
@@ -1713,17 +1689,13 @@
         <v>34</v>
       </c>
       <c r="D26" s="59"/>
-      <c r="E26" s="78"/>
-      <c r="F26" s="79"/>
+      <c r="E26" s="103"/>
+      <c r="F26" s="104"/>
       <c r="G26" s="52"/>
-      <c r="H26" s="85"/>
-      <c r="I26" s="86"/>
-      <c r="K26" s="44">
-        <v>2289</v>
-      </c>
-      <c r="L26" s="44">
-        <v>2520</v>
-      </c>
+      <c r="H26" s="99"/>
+      <c r="I26" s="100"/>
+      <c r="K26" s="44"/>
+      <c r="L26" s="44"/>
       <c r="M26" s="45"/>
       <c r="N26" s="23"/>
       <c r="Q26" s="13"/>
@@ -1738,17 +1710,13 @@
         <v>29</v>
       </c>
       <c r="D27" s="61"/>
-      <c r="E27" s="80"/>
-      <c r="F27" s="81"/>
+      <c r="E27" s="97"/>
+      <c r="F27" s="98"/>
       <c r="G27" s="52"/>
-      <c r="H27" s="85"/>
-      <c r="I27" s="86"/>
-      <c r="K27" s="60">
-        <v>0.05</v>
-      </c>
-      <c r="L27" s="60">
-        <v>0.99</v>
-      </c>
+      <c r="H27" s="99"/>
+      <c r="I27" s="100"/>
+      <c r="K27" s="60"/>
+      <c r="L27" s="60"/>
       <c r="M27" s="45"/>
       <c r="N27" s="23"/>
       <c r="Q27" s="13"/>
@@ -1763,17 +1731,13 @@
         <v>29</v>
       </c>
       <c r="D28" s="65"/>
-      <c r="E28" s="80"/>
-      <c r="F28" s="81"/>
+      <c r="E28" s="97"/>
+      <c r="F28" s="98"/>
       <c r="G28" s="52"/>
-      <c r="H28" s="85"/>
-      <c r="I28" s="86"/>
-      <c r="K28" s="44">
-        <v>2.5</v>
-      </c>
-      <c r="L28" s="44">
-        <v>4.5</v>
-      </c>
+      <c r="H28" s="99"/>
+      <c r="I28" s="100"/>
+      <c r="K28" s="44"/>
+      <c r="L28" s="44"/>
       <c r="M28" s="45"/>
       <c r="N28" s="23"/>
       <c r="Y28" s="49"/>
@@ -1787,17 +1751,13 @@
         <v>38</v>
       </c>
       <c r="D29" s="65"/>
-      <c r="E29" s="80"/>
-      <c r="F29" s="81"/>
+      <c r="E29" s="97"/>
+      <c r="F29" s="98"/>
       <c r="G29" s="52"/>
-      <c r="H29" s="85"/>
-      <c r="I29" s="86"/>
-      <c r="K29" s="44">
-        <v>3</v>
-      </c>
-      <c r="L29" s="44">
-        <v>12</v>
-      </c>
+      <c r="H29" s="99"/>
+      <c r="I29" s="100"/>
+      <c r="K29" s="44"/>
+      <c r="L29" s="44"/>
       <c r="M29" s="45"/>
       <c r="N29" s="23"/>
       <c r="Y29" s="50"/>
@@ -1806,12 +1766,12 @@
       <c r="A30" s="66" t="s">
         <v>39</v>
       </c>
-      <c r="B30" s="82"/>
-      <c r="C30" s="82"/>
-      <c r="D30" s="82"/>
-      <c r="E30" s="82"/>
-      <c r="F30" s="82"/>
-      <c r="G30" s="82"/>
+      <c r="B30" s="94"/>
+      <c r="C30" s="94"/>
+      <c r="D30" s="94"/>
+      <c r="E30" s="94"/>
+      <c r="F30" s="94"/>
+      <c r="G30" s="94"/>
       <c r="H30" s="67"/>
       <c r="I30" s="67"/>
       <c r="Y30" s="50"/>
@@ -1891,15 +1851,11 @@
     <protectedRange sqref="E10" name="Range1_3"/>
   </protectedRanges>
   <mergeCells count="30">
-    <mergeCell ref="E12:H13"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="Y17:Y19"/>
-    <mergeCell ref="A18:C19"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="E18:F19"/>
-    <mergeCell ref="G18:G19"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E29:F29"/>
     <mergeCell ref="B30:G30"/>
     <mergeCell ref="H20:I20"/>
     <mergeCell ref="H21:I21"/>
@@ -1916,11 +1872,15 @@
     <mergeCell ref="E22:F22"/>
     <mergeCell ref="E23:F23"/>
     <mergeCell ref="E24:F24"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="E12:H13"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="Y17:Y19"/>
+    <mergeCell ref="A18:C19"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="E18:F19"/>
+    <mergeCell ref="G18:G19"/>
   </mergeCells>
   <conditionalFormatting sqref="I12:I16 E12 E14:H16">
     <cfRule type="cellIs" dxfId="1" priority="2" stopIfTrue="1" operator="equal">

</xml_diff>

<commit_message>
M3 QA Cord #548 - Fixed COA1   - Change Label (NO -> NO.)   - DENIER     - Change MIN. to Min.     - Result convert to integer Floor mode   - RPU     - Result has 2 decimal places.
</commit_message>
<xml_diff>
--- a/05.Controls/M3.QA.Controls/Resources/Excels/COA1.xlsx
+++ b/05.Controls/M3.QA.Controls/Resources/Excels/COA1.xlsx
@@ -176,9 +176,6 @@
     <t>MOISTURE REGAIN</t>
   </si>
   <si>
-    <t>RPU</t>
-  </si>
-  <si>
     <t>ADHESION FORCE (PEEL)</t>
   </si>
   <si>
@@ -203,7 +200,10 @@
     <t>SHRINKAGE</t>
   </si>
   <si>
-    <t>TWISTING NO</t>
+    <t>TWISTING NO.</t>
+  </si>
+  <si>
+    <t>RPU.</t>
   </si>
 </sst>
 </file>
@@ -756,6 +756,39 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="5" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -809,39 +842,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="11">
@@ -910,7 +910,7 @@
         <xdr:cNvPr id="2" name="Picture 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8C6984C9-0C37-400A-AFFE-0753047B13B4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{8C6984C9-0C37-400A-AFFE-0753047B13B4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1236,7 +1236,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1246,8 +1246,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Y36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.5546875" defaultRowHeight="13.2"/>
@@ -1431,10 +1431,10 @@
       <c r="B12" s="19"/>
       <c r="C12" s="13"/>
       <c r="D12" s="13"/>
-      <c r="E12" s="76"/>
-      <c r="F12" s="77"/>
-      <c r="G12" s="77"/>
-      <c r="H12" s="78"/>
+      <c r="E12" s="87"/>
+      <c r="F12" s="88"/>
+      <c r="G12" s="88"/>
+      <c r="H12" s="89"/>
       <c r="I12" s="20"/>
       <c r="N12" s="74"/>
     </row>
@@ -1445,10 +1445,10 @@
       <c r="B13" s="21"/>
       <c r="C13" s="22"/>
       <c r="D13" s="13"/>
-      <c r="E13" s="79"/>
-      <c r="F13" s="80"/>
-      <c r="G13" s="80"/>
-      <c r="H13" s="81"/>
+      <c r="E13" s="90"/>
+      <c r="F13" s="91"/>
+      <c r="G13" s="91"/>
+      <c r="H13" s="92"/>
       <c r="I13" s="20"/>
       <c r="K13" s="23"/>
       <c r="N13" s="74"/>
@@ -1460,14 +1460,14 @@
       <c r="B14" s="24"/>
       <c r="C14" s="13"/>
       <c r="D14" s="13"/>
-      <c r="E14" s="82" t="s">
+      <c r="E14" s="93" t="s">
         <v>13</v>
       </c>
-      <c r="F14" s="83"/>
-      <c r="G14" s="82" t="s">
+      <c r="F14" s="94"/>
+      <c r="G14" s="93" t="s">
         <v>14</v>
       </c>
-      <c r="H14" s="83"/>
+      <c r="H14" s="94"/>
       <c r="I14" s="25" t="s">
         <v>15</v>
       </c>
@@ -1477,8 +1477,8 @@
       <c r="A15" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="84"/>
-      <c r="C15" s="84"/>
+      <c r="B15" s="95"/>
+      <c r="C15" s="95"/>
       <c r="D15" s="13"/>
       <c r="E15" s="26"/>
       <c r="F15" s="27"/>
@@ -1516,22 +1516,22 @@
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
       <c r="N17" s="74"/>
-      <c r="Y17" s="85"/>
+      <c r="Y17" s="96"/>
     </row>
     <row r="18" spans="1:25" ht="19.8">
-      <c r="A18" s="86" t="s">
+      <c r="A18" s="97" t="s">
         <v>20</v>
       </c>
-      <c r="B18" s="87"/>
-      <c r="C18" s="88"/>
-      <c r="D18" s="92" t="s">
+      <c r="B18" s="98"/>
+      <c r="C18" s="99"/>
+      <c r="D18" s="103" t="s">
         <v>21</v>
       </c>
-      <c r="E18" s="86" t="s">
+      <c r="E18" s="97" t="s">
         <v>22</v>
       </c>
-      <c r="F18" s="88"/>
-      <c r="G18" s="92" t="s">
+      <c r="F18" s="99"/>
+      <c r="G18" s="103" t="s">
         <v>23</v>
       </c>
       <c r="H18" s="34" t="s">
@@ -1541,16 +1541,16 @@
       <c r="N18" s="74"/>
       <c r="Q18" s="13"/>
       <c r="T18" s="36"/>
-      <c r="Y18" s="85"/>
+      <c r="Y18" s="96"/>
     </row>
     <row r="19" spans="1:25" ht="21.6">
-      <c r="A19" s="89"/>
-      <c r="B19" s="90"/>
-      <c r="C19" s="91"/>
-      <c r="D19" s="93"/>
-      <c r="E19" s="89"/>
-      <c r="F19" s="91"/>
-      <c r="G19" s="93"/>
+      <c r="A19" s="100"/>
+      <c r="B19" s="101"/>
+      <c r="C19" s="102"/>
+      <c r="D19" s="104"/>
+      <c r="E19" s="100"/>
+      <c r="F19" s="102"/>
+      <c r="G19" s="104"/>
       <c r="H19" s="37" t="s">
         <v>25</v>
       </c>
@@ -1560,7 +1560,7 @@
       <c r="M19" s="23"/>
       <c r="Q19" s="13"/>
       <c r="T19" s="36"/>
-      <c r="Y19" s="85"/>
+      <c r="Y19" s="96"/>
     </row>
     <row r="20" spans="1:25" ht="19.8">
       <c r="A20" s="39" t="s">
@@ -1571,11 +1571,11 @@
         <v>27</v>
       </c>
       <c r="D20" s="42"/>
-      <c r="E20" s="101"/>
-      <c r="F20" s="102"/>
+      <c r="E20" s="76"/>
+      <c r="F20" s="77"/>
       <c r="G20" s="43"/>
-      <c r="H20" s="95"/>
-      <c r="I20" s="96"/>
+      <c r="H20" s="83"/>
+      <c r="I20" s="84"/>
       <c r="K20" s="44"/>
       <c r="L20" s="44"/>
       <c r="M20" s="45"/>
@@ -1591,11 +1591,11 @@
         <v>29</v>
       </c>
       <c r="D21" s="48"/>
-      <c r="E21" s="101"/>
-      <c r="F21" s="102"/>
+      <c r="E21" s="76"/>
+      <c r="F21" s="77"/>
       <c r="G21" s="43"/>
-      <c r="H21" s="95"/>
-      <c r="I21" s="96"/>
+      <c r="H21" s="83"/>
+      <c r="I21" s="84"/>
       <c r="K21" s="44"/>
       <c r="L21" s="44"/>
       <c r="M21" s="45"/>
@@ -1612,11 +1612,11 @@
         <v>29</v>
       </c>
       <c r="D22" s="51"/>
-      <c r="E22" s="101"/>
-      <c r="F22" s="102"/>
+      <c r="E22" s="76"/>
+      <c r="F22" s="77"/>
       <c r="G22" s="52"/>
-      <c r="H22" s="95"/>
-      <c r="I22" s="96"/>
+      <c r="H22" s="83"/>
+      <c r="I22" s="84"/>
       <c r="K22" s="44"/>
       <c r="L22" s="44"/>
       <c r="M22" s="45"/>
@@ -1625,18 +1625,18 @@
     </row>
     <row r="23" spans="1:25" ht="24.75" customHeight="1">
       <c r="A23" s="53" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="54" t="s">
         <v>31</v>
       </c>
       <c r="D23" s="55"/>
-      <c r="E23" s="101"/>
-      <c r="F23" s="102"/>
+      <c r="E23" s="76"/>
+      <c r="F23" s="77"/>
       <c r="G23" s="52"/>
-      <c r="H23" s="95"/>
-      <c r="I23" s="96"/>
+      <c r="H23" s="83"/>
+      <c r="I23" s="84"/>
       <c r="K23" s="44"/>
       <c r="L23" s="44"/>
       <c r="M23" s="45"/>
@@ -1651,11 +1651,11 @@
         <v>33</v>
       </c>
       <c r="D24" s="59"/>
-      <c r="E24" s="97"/>
-      <c r="F24" s="98"/>
+      <c r="E24" s="80"/>
+      <c r="F24" s="81"/>
       <c r="G24" s="52"/>
-      <c r="H24" s="95"/>
-      <c r="I24" s="96"/>
+      <c r="H24" s="83"/>
+      <c r="I24" s="84"/>
       <c r="K24" s="60"/>
       <c r="L24" s="60"/>
       <c r="M24" s="45"/>
@@ -1663,18 +1663,18 @@
     </row>
     <row r="25" spans="1:25" ht="19.8">
       <c r="A25" s="39" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B25" s="40"/>
       <c r="C25" s="41" t="s">
         <v>29</v>
       </c>
       <c r="D25" s="61"/>
-      <c r="E25" s="101"/>
-      <c r="F25" s="102"/>
+      <c r="E25" s="76"/>
+      <c r="F25" s="77"/>
       <c r="G25" s="52"/>
-      <c r="H25" s="97"/>
-      <c r="I25" s="98"/>
+      <c r="H25" s="80"/>
+      <c r="I25" s="81"/>
       <c r="K25" s="44"/>
       <c r="L25" s="44"/>
       <c r="M25" s="45"/>
@@ -1682,18 +1682,18 @@
     </row>
     <row r="26" spans="1:25" ht="19.8">
       <c r="A26" s="62" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B26" s="13"/>
       <c r="C26" s="54" t="s">
         <v>34</v>
       </c>
       <c r="D26" s="59"/>
-      <c r="E26" s="103"/>
-      <c r="F26" s="104"/>
+      <c r="E26" s="78"/>
+      <c r="F26" s="79"/>
       <c r="G26" s="52"/>
-      <c r="H26" s="99"/>
-      <c r="I26" s="100"/>
+      <c r="H26" s="85"/>
+      <c r="I26" s="86"/>
       <c r="K26" s="44"/>
       <c r="L26" s="44"/>
       <c r="M26" s="45"/>
@@ -1710,11 +1710,11 @@
         <v>29</v>
       </c>
       <c r="D27" s="61"/>
-      <c r="E27" s="97"/>
-      <c r="F27" s="98"/>
+      <c r="E27" s="80"/>
+      <c r="F27" s="81"/>
       <c r="G27" s="52"/>
-      <c r="H27" s="99"/>
-      <c r="I27" s="100"/>
+      <c r="H27" s="85"/>
+      <c r="I27" s="86"/>
       <c r="K27" s="60"/>
       <c r="L27" s="60"/>
       <c r="M27" s="45"/>
@@ -1724,18 +1724,18 @@
     </row>
     <row r="28" spans="1:25" ht="19.8">
       <c r="A28" s="39" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="B28" s="40"/>
       <c r="C28" s="41" t="s">
         <v>29</v>
       </c>
       <c r="D28" s="65"/>
-      <c r="E28" s="97"/>
-      <c r="F28" s="98"/>
+      <c r="E28" s="80"/>
+      <c r="F28" s="81"/>
       <c r="G28" s="52"/>
-      <c r="H28" s="99"/>
-      <c r="I28" s="100"/>
+      <c r="H28" s="85"/>
+      <c r="I28" s="86"/>
       <c r="K28" s="44"/>
       <c r="L28" s="44"/>
       <c r="M28" s="45"/>
@@ -1744,18 +1744,18 @@
     </row>
     <row r="29" spans="1:25" ht="19.8">
       <c r="A29" s="39" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B29" s="40"/>
       <c r="C29" s="41" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D29" s="65"/>
-      <c r="E29" s="97"/>
-      <c r="F29" s="98"/>
+      <c r="E29" s="80"/>
+      <c r="F29" s="81"/>
       <c r="G29" s="52"/>
-      <c r="H29" s="99"/>
-      <c r="I29" s="100"/>
+      <c r="H29" s="85"/>
+      <c r="I29" s="86"/>
       <c r="K29" s="44"/>
       <c r="L29" s="44"/>
       <c r="M29" s="45"/>
@@ -1764,14 +1764,14 @@
     </row>
     <row r="30" spans="1:25" ht="25.5" customHeight="1">
       <c r="A30" s="66" t="s">
-        <v>39</v>
-      </c>
-      <c r="B30" s="94"/>
-      <c r="C30" s="94"/>
-      <c r="D30" s="94"/>
-      <c r="E30" s="94"/>
-      <c r="F30" s="94"/>
-      <c r="G30" s="94"/>
+        <v>38</v>
+      </c>
+      <c r="B30" s="82"/>
+      <c r="C30" s="82"/>
+      <c r="D30" s="82"/>
+      <c r="E30" s="82"/>
+      <c r="F30" s="82"/>
+      <c r="G30" s="82"/>
       <c r="H30" s="67"/>
       <c r="I30" s="67"/>
       <c r="Y30" s="50"/>
@@ -1789,7 +1789,7 @@
     </row>
     <row r="32" spans="1:25" ht="19.8">
       <c r="A32" s="69" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B32" s="70"/>
       <c r="C32" s="70"/>
@@ -1813,7 +1813,7 @@
     </row>
     <row r="34" spans="1:9" ht="17.399999999999999">
       <c r="A34" s="71" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B34" s="71"/>
       <c r="C34" s="71"/>
@@ -1821,7 +1821,7 @@
       <c r="E34" s="71"/>
       <c r="H34" s="72"/>
       <c r="I34" s="72" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="35" spans="1:9" ht="19.8">
@@ -1851,11 +1851,15 @@
     <protectedRange sqref="E10" name="Range1_3"/>
   </protectedRanges>
   <mergeCells count="30">
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="E12:H13"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="Y17:Y19"/>
+    <mergeCell ref="A18:C19"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="E18:F19"/>
+    <mergeCell ref="G18:G19"/>
     <mergeCell ref="B30:G30"/>
     <mergeCell ref="H20:I20"/>
     <mergeCell ref="H21:I21"/>
@@ -1872,15 +1876,11 @@
     <mergeCell ref="E22:F22"/>
     <mergeCell ref="E23:F23"/>
     <mergeCell ref="E24:F24"/>
-    <mergeCell ref="E12:H13"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="Y17:Y19"/>
-    <mergeCell ref="A18:C19"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="E18:F19"/>
-    <mergeCell ref="G18:G19"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E29:F29"/>
   </mergeCells>
   <conditionalFormatting sqref="I12:I16 E12 E14:H16">
     <cfRule type="cellIs" dxfId="1" priority="2" stopIfTrue="1" operator="equal">

</xml_diff>

<commit_message>
M3 QA Cord #551 - Coa1, Coa1a update math calculation Floor with supports decimal places.
</commit_message>
<xml_diff>
--- a/05.Controls/M3.QA.Controls/Resources/Excels/COA1.xlsx
+++ b/05.Controls/M3.QA.Controls/Resources/Excels/COA1.xlsx
@@ -586,9 +586,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
@@ -756,6 +753,81 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="5" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="167" fontId="3" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -768,80 +840,8 @@
     <xf numFmtId="1" fontId="3" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="5" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="11">
@@ -910,7 +910,7 @@
         <xdr:cNvPr id="2" name="Picture 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{8C6984C9-0C37-400A-AFFE-0753047B13B4}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8C6984C9-0C37-400A-AFFE-0753047B13B4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1236,7 +1236,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1246,8 +1246,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Y36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.5546875" defaultRowHeight="13.2"/>
@@ -1260,7 +1260,7 @@
     <col min="10" max="13" width="7.5546875" style="2"/>
     <col min="14" max="14" width="10.44140625" style="2" customWidth="1"/>
     <col min="15" max="24" width="7.5546875" style="2"/>
-    <col min="25" max="25" width="7.5546875" style="47"/>
+    <col min="25" max="25" width="7.5546875" style="46"/>
     <col min="26" max="16384" width="7.5546875" style="2"/>
   </cols>
   <sheetData>
@@ -1274,7 +1274,7 @@
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
-      <c r="N1" s="73"/>
+      <c r="N1" s="72"/>
     </row>
     <row r="2" spans="1:23" ht="14.25" customHeight="1">
       <c r="A2" s="3" t="s">
@@ -1288,7 +1288,7 @@
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
-      <c r="N2" s="74"/>
+      <c r="N2" s="73"/>
     </row>
     <row r="3" spans="1:23" ht="14.25" customHeight="1">
       <c r="A3" s="3" t="s">
@@ -1302,7 +1302,7 @@
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
-      <c r="N3" s="74"/>
+      <c r="N3" s="73"/>
     </row>
     <row r="4" spans="1:23" ht="14.25" customHeight="1">
       <c r="A4" s="3" t="s">
@@ -1316,7 +1316,7 @@
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
-      <c r="N4" s="74"/>
+      <c r="N4" s="73"/>
       <c r="W4" s="4"/>
     </row>
     <row r="5" spans="1:23" ht="14.25" customHeight="1">
@@ -1331,7 +1331,7 @@
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
-      <c r="N5" s="74"/>
+      <c r="N5" s="73"/>
     </row>
     <row r="6" spans="1:23" ht="14.25" customHeight="1">
       <c r="A6" s="5" t="s">
@@ -1345,7 +1345,7 @@
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
-      <c r="N6" s="74"/>
+      <c r="N6" s="73"/>
     </row>
     <row r="7" spans="1:23" ht="20.399999999999999">
       <c r="A7" s="5"/>
@@ -1364,7 +1364,7 @@
       <c r="J7" s="9"/>
       <c r="K7" s="9"/>
       <c r="L7" s="9"/>
-      <c r="N7" s="74"/>
+      <c r="N7" s="73"/>
     </row>
     <row r="8" spans="1:23" ht="19.8">
       <c r="A8" s="1"/>
@@ -1376,7 +1376,7 @@
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
-      <c r="N8" s="74"/>
+      <c r="N8" s="73"/>
     </row>
     <row r="9" spans="1:23" ht="26.4">
       <c r="A9" s="10" t="s">
@@ -1390,7 +1390,7 @@
       <c r="G9" s="6"/>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
-      <c r="N9" s="75"/>
+      <c r="N9" s="74"/>
     </row>
     <row r="10" spans="1:23" ht="19.8">
       <c r="A10" s="1"/>
@@ -1404,104 +1404,104 @@
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
-      <c r="N10" s="74"/>
+      <c r="N10" s="73"/>
     </row>
     <row r="11" spans="1:23" ht="22.5" customHeight="1">
       <c r="A11" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="14"/>
+      <c r="B11" s="104"/>
       <c r="C11" s="13"/>
       <c r="D11" s="13"/>
-      <c r="E11" s="15" t="s">
+      <c r="E11" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="F11" s="16"/>
-      <c r="G11" s="16"/>
-      <c r="H11" s="17"/>
-      <c r="I11" s="18" t="s">
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="N11" s="74"/>
+      <c r="N11" s="73"/>
     </row>
     <row r="12" spans="1:23" ht="22.5" customHeight="1">
       <c r="A12" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="19"/>
+      <c r="B12" s="18"/>
       <c r="C12" s="13"/>
       <c r="D12" s="13"/>
-      <c r="E12" s="87"/>
-      <c r="F12" s="88"/>
-      <c r="G12" s="88"/>
-      <c r="H12" s="89"/>
-      <c r="I12" s="20"/>
-      <c r="N12" s="74"/>
+      <c r="E12" s="75"/>
+      <c r="F12" s="76"/>
+      <c r="G12" s="76"/>
+      <c r="H12" s="77"/>
+      <c r="I12" s="19"/>
+      <c r="N12" s="73"/>
     </row>
     <row r="13" spans="1:23" ht="22.5" customHeight="1">
       <c r="A13" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="21"/>
-      <c r="C13" s="22"/>
+      <c r="B13" s="20"/>
+      <c r="C13" s="21"/>
       <c r="D13" s="13"/>
-      <c r="E13" s="90"/>
-      <c r="F13" s="91"/>
-      <c r="G13" s="91"/>
-      <c r="H13" s="92"/>
-      <c r="I13" s="20"/>
-      <c r="K13" s="23"/>
-      <c r="N13" s="74"/>
+      <c r="E13" s="78"/>
+      <c r="F13" s="79"/>
+      <c r="G13" s="79"/>
+      <c r="H13" s="80"/>
+      <c r="I13" s="19"/>
+      <c r="K13" s="22"/>
+      <c r="N13" s="73"/>
     </row>
     <row r="14" spans="1:23" ht="22.5" customHeight="1">
       <c r="A14" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="24"/>
+      <c r="B14" s="23"/>
       <c r="C14" s="13"/>
       <c r="D14" s="13"/>
-      <c r="E14" s="93" t="s">
+      <c r="E14" s="81" t="s">
         <v>13</v>
       </c>
-      <c r="F14" s="94"/>
-      <c r="G14" s="93" t="s">
+      <c r="F14" s="82"/>
+      <c r="G14" s="81" t="s">
         <v>14</v>
       </c>
-      <c r="H14" s="94"/>
-      <c r="I14" s="25" t="s">
+      <c r="H14" s="82"/>
+      <c r="I14" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="N14" s="74"/>
+      <c r="N14" s="73"/>
     </row>
     <row r="15" spans="1:23" ht="22.5" customHeight="1">
       <c r="A15" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="95"/>
-      <c r="C15" s="95"/>
+      <c r="B15" s="83"/>
+      <c r="C15" s="83"/>
       <c r="D15" s="13"/>
-      <c r="E15" s="26"/>
-      <c r="F15" s="27"/>
-      <c r="G15" s="26"/>
-      <c r="H15" s="28"/>
-      <c r="I15" s="20"/>
-      <c r="N15" s="74"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="26"/>
+      <c r="G15" s="25"/>
+      <c r="H15" s="27"/>
+      <c r="I15" s="19"/>
+      <c r="N15" s="73"/>
     </row>
     <row r="16" spans="1:23" ht="22.5" customHeight="1">
       <c r="A16" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="29"/>
-      <c r="C16" s="24" t="s">
+      <c r="B16" s="28"/>
+      <c r="C16" s="23" t="s">
         <v>18</v>
       </c>
       <c r="D16" s="13"/>
-      <c r="E16" s="30"/>
-      <c r="F16" s="31"/>
-      <c r="G16" s="30"/>
-      <c r="H16" s="32"/>
-      <c r="I16" s="33"/>
-      <c r="N16" s="74"/>
+      <c r="E16" s="29"/>
+      <c r="F16" s="30"/>
+      <c r="G16" s="29"/>
+      <c r="H16" s="31"/>
+      <c r="I16" s="32"/>
+      <c r="N16" s="73"/>
     </row>
     <row r="17" spans="1:25" ht="19.8">
       <c r="A17" s="1" t="s">
@@ -1515,284 +1515,284 @@
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
-      <c r="N17" s="74"/>
-      <c r="Y17" s="96"/>
+      <c r="N17" s="73"/>
+      <c r="Y17" s="84"/>
     </row>
     <row r="18" spans="1:25" ht="19.8">
-      <c r="A18" s="97" t="s">
+      <c r="A18" s="85" t="s">
         <v>20</v>
       </c>
-      <c r="B18" s="98"/>
-      <c r="C18" s="99"/>
-      <c r="D18" s="103" t="s">
+      <c r="B18" s="86"/>
+      <c r="C18" s="87"/>
+      <c r="D18" s="91" t="s">
         <v>21</v>
       </c>
-      <c r="E18" s="97" t="s">
+      <c r="E18" s="85" t="s">
         <v>22</v>
       </c>
-      <c r="F18" s="99"/>
-      <c r="G18" s="103" t="s">
+      <c r="F18" s="87"/>
+      <c r="G18" s="91" t="s">
         <v>23</v>
       </c>
-      <c r="H18" s="34" t="s">
+      <c r="H18" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="I18" s="35"/>
-      <c r="N18" s="74"/>
+      <c r="I18" s="34"/>
+      <c r="N18" s="73"/>
       <c r="Q18" s="13"/>
-      <c r="T18" s="36"/>
-      <c r="Y18" s="96"/>
+      <c r="T18" s="35"/>
+      <c r="Y18" s="84"/>
     </row>
     <row r="19" spans="1:25" ht="21.6">
-      <c r="A19" s="100"/>
-      <c r="B19" s="101"/>
-      <c r="C19" s="102"/>
-      <c r="D19" s="104"/>
-      <c r="E19" s="100"/>
-      <c r="F19" s="102"/>
-      <c r="G19" s="104"/>
-      <c r="H19" s="37" t="s">
+      <c r="A19" s="88"/>
+      <c r="B19" s="89"/>
+      <c r="C19" s="90"/>
+      <c r="D19" s="92"/>
+      <c r="E19" s="88"/>
+      <c r="F19" s="90"/>
+      <c r="G19" s="92"/>
+      <c r="H19" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="I19" s="38"/>
-      <c r="K19" s="23"/>
-      <c r="L19" s="23"/>
-      <c r="M19" s="23"/>
+      <c r="I19" s="37"/>
+      <c r="K19" s="22"/>
+      <c r="L19" s="22"/>
+      <c r="M19" s="22"/>
       <c r="Q19" s="13"/>
-      <c r="T19" s="36"/>
-      <c r="Y19" s="96"/>
+      <c r="T19" s="35"/>
+      <c r="Y19" s="84"/>
     </row>
     <row r="20" spans="1:25" ht="19.8">
-      <c r="A20" s="39" t="s">
+      <c r="A20" s="38" t="s">
         <v>26</v>
       </c>
-      <c r="B20" s="40"/>
-      <c r="C20" s="41" t="s">
+      <c r="B20" s="39"/>
+      <c r="C20" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="D20" s="42"/>
-      <c r="E20" s="76"/>
-      <c r="F20" s="77"/>
-      <c r="G20" s="43"/>
-      <c r="H20" s="83"/>
-      <c r="I20" s="84"/>
-      <c r="K20" s="44"/>
-      <c r="L20" s="44"/>
-      <c r="M20" s="45"/>
+      <c r="D20" s="41"/>
+      <c r="E20" s="100"/>
+      <c r="F20" s="101"/>
+      <c r="G20" s="42"/>
+      <c r="H20" s="94"/>
+      <c r="I20" s="95"/>
+      <c r="K20" s="43"/>
+      <c r="L20" s="43"/>
+      <c r="M20" s="44"/>
       <c r="Q20" s="13"/>
-      <c r="T20" s="46"/>
+      <c r="T20" s="45"/>
     </row>
     <row r="21" spans="1:25" ht="19.8">
-      <c r="A21" s="39" t="s">
+      <c r="A21" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="B21" s="40"/>
-      <c r="C21" s="41" t="s">
+      <c r="B21" s="39"/>
+      <c r="C21" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="D21" s="48"/>
-      <c r="E21" s="76"/>
-      <c r="F21" s="77"/>
-      <c r="G21" s="43"/>
-      <c r="H21" s="83"/>
-      <c r="I21" s="84"/>
-      <c r="K21" s="44"/>
-      <c r="L21" s="44"/>
-      <c r="M21" s="45"/>
+      <c r="D21" s="47"/>
+      <c r="E21" s="100"/>
+      <c r="F21" s="101"/>
+      <c r="G21" s="42"/>
+      <c r="H21" s="94"/>
+      <c r="I21" s="95"/>
+      <c r="K21" s="43"/>
+      <c r="L21" s="43"/>
+      <c r="M21" s="44"/>
       <c r="Q21" s="1"/>
-      <c r="T21" s="49"/>
-      <c r="Y21" s="50"/>
+      <c r="T21" s="48"/>
+      <c r="Y21" s="49"/>
     </row>
     <row r="22" spans="1:25" ht="19.8">
-      <c r="A22" s="39" t="s">
+      <c r="A22" s="38" t="s">
         <v>30</v>
       </c>
-      <c r="B22" s="40"/>
-      <c r="C22" s="41" t="s">
+      <c r="B22" s="39"/>
+      <c r="C22" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="D22" s="51"/>
-      <c r="E22" s="76"/>
-      <c r="F22" s="77"/>
-      <c r="G22" s="52"/>
-      <c r="H22" s="83"/>
-      <c r="I22" s="84"/>
-      <c r="K22" s="44"/>
-      <c r="L22" s="44"/>
-      <c r="M22" s="45"/>
+      <c r="D22" s="50"/>
+      <c r="E22" s="100"/>
+      <c r="F22" s="101"/>
+      <c r="G22" s="51"/>
+      <c r="H22" s="94"/>
+      <c r="I22" s="95"/>
+      <c r="K22" s="43"/>
+      <c r="L22" s="43"/>
+      <c r="M22" s="44"/>
       <c r="Q22" s="1"/>
-      <c r="Y22" s="49"/>
+      <c r="Y22" s="48"/>
     </row>
     <row r="23" spans="1:25" ht="24.75" customHeight="1">
-      <c r="A23" s="53" t="s">
+      <c r="A23" s="52" t="s">
         <v>44</v>
       </c>
       <c r="B23" s="1"/>
-      <c r="C23" s="54" t="s">
+      <c r="C23" s="53" t="s">
         <v>31</v>
       </c>
-      <c r="D23" s="55"/>
-      <c r="E23" s="76"/>
-      <c r="F23" s="77"/>
-      <c r="G23" s="52"/>
-      <c r="H23" s="83"/>
-      <c r="I23" s="84"/>
-      <c r="K23" s="44"/>
-      <c r="L23" s="44"/>
-      <c r="M23" s="45"/>
+      <c r="D23" s="54"/>
+      <c r="E23" s="100"/>
+      <c r="F23" s="101"/>
+      <c r="G23" s="51"/>
+      <c r="H23" s="94"/>
+      <c r="I23" s="95"/>
+      <c r="K23" s="43"/>
+      <c r="L23" s="43"/>
+      <c r="M23" s="44"/>
       <c r="Q23" s="13"/>
     </row>
     <row r="24" spans="1:25" ht="19.8">
-      <c r="A24" s="56" t="s">
+      <c r="A24" s="55" t="s">
         <v>32</v>
       </c>
-      <c r="B24" s="57"/>
-      <c r="C24" s="58" t="s">
+      <c r="B24" s="56"/>
+      <c r="C24" s="57" t="s">
         <v>33</v>
       </c>
-      <c r="D24" s="59"/>
-      <c r="E24" s="80"/>
-      <c r="F24" s="81"/>
-      <c r="G24" s="52"/>
-      <c r="H24" s="83"/>
-      <c r="I24" s="84"/>
-      <c r="K24" s="60"/>
-      <c r="L24" s="60"/>
-      <c r="M24" s="45"/>
+      <c r="D24" s="58"/>
+      <c r="E24" s="96"/>
+      <c r="F24" s="97"/>
+      <c r="G24" s="51"/>
+      <c r="H24" s="94"/>
+      <c r="I24" s="95"/>
+      <c r="K24" s="59"/>
+      <c r="L24" s="59"/>
+      <c r="M24" s="44"/>
       <c r="Q24" s="13"/>
     </row>
     <row r="25" spans="1:25" ht="19.8">
-      <c r="A25" s="39" t="s">
+      <c r="A25" s="38" t="s">
         <v>43</v>
       </c>
-      <c r="B25" s="40"/>
-      <c r="C25" s="41" t="s">
+      <c r="B25" s="39"/>
+      <c r="C25" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="D25" s="61"/>
-      <c r="E25" s="76"/>
-      <c r="F25" s="77"/>
-      <c r="G25" s="52"/>
-      <c r="H25" s="80"/>
-      <c r="I25" s="81"/>
-      <c r="K25" s="44"/>
-      <c r="L25" s="44"/>
-      <c r="M25" s="45"/>
+      <c r="D25" s="60"/>
+      <c r="E25" s="100"/>
+      <c r="F25" s="101"/>
+      <c r="G25" s="51"/>
+      <c r="H25" s="96"/>
+      <c r="I25" s="97"/>
+      <c r="K25" s="43"/>
+      <c r="L25" s="43"/>
+      <c r="M25" s="44"/>
       <c r="Q25" s="13"/>
     </row>
     <row r="26" spans="1:25" ht="19.8">
-      <c r="A26" s="62" t="s">
+      <c r="A26" s="61" t="s">
         <v>42</v>
       </c>
       <c r="B26" s="13"/>
-      <c r="C26" s="54" t="s">
+      <c r="C26" s="53" t="s">
         <v>34</v>
       </c>
-      <c r="D26" s="59"/>
-      <c r="E26" s="78"/>
-      <c r="F26" s="79"/>
-      <c r="G26" s="52"/>
-      <c r="H26" s="85"/>
-      <c r="I26" s="86"/>
-      <c r="K26" s="44"/>
-      <c r="L26" s="44"/>
-      <c r="M26" s="45"/>
-      <c r="N26" s="23"/>
+      <c r="D26" s="58"/>
+      <c r="E26" s="102"/>
+      <c r="F26" s="103"/>
+      <c r="G26" s="51"/>
+      <c r="H26" s="98"/>
+      <c r="I26" s="99"/>
+      <c r="K26" s="43"/>
+      <c r="L26" s="43"/>
+      <c r="M26" s="44"/>
+      <c r="N26" s="22"/>
       <c r="Q26" s="13"/>
-      <c r="T26" s="49"/>
+      <c r="T26" s="48"/>
     </row>
     <row r="27" spans="1:25" ht="19.8">
-      <c r="A27" s="63" t="s">
+      <c r="A27" s="62" t="s">
         <v>35</v>
       </c>
-      <c r="B27" s="64"/>
-      <c r="C27" s="58" t="s">
+      <c r="B27" s="63"/>
+      <c r="C27" s="57" t="s">
         <v>29</v>
       </c>
-      <c r="D27" s="61"/>
-      <c r="E27" s="80"/>
-      <c r="F27" s="81"/>
-      <c r="G27" s="52"/>
-      <c r="H27" s="85"/>
-      <c r="I27" s="86"/>
-      <c r="K27" s="60"/>
-      <c r="L27" s="60"/>
-      <c r="M27" s="45"/>
-      <c r="N27" s="23"/>
+      <c r="D27" s="60"/>
+      <c r="E27" s="96"/>
+      <c r="F27" s="97"/>
+      <c r="G27" s="51"/>
+      <c r="H27" s="98"/>
+      <c r="I27" s="99"/>
+      <c r="K27" s="59"/>
+      <c r="L27" s="59"/>
+      <c r="M27" s="44"/>
+      <c r="N27" s="22"/>
       <c r="Q27" s="13"/>
-      <c r="T27" s="46"/>
+      <c r="T27" s="45"/>
     </row>
     <row r="28" spans="1:25" ht="19.8">
-      <c r="A28" s="39" t="s">
+      <c r="A28" s="38" t="s">
         <v>45</v>
       </c>
-      <c r="B28" s="40"/>
-      <c r="C28" s="41" t="s">
+      <c r="B28" s="39"/>
+      <c r="C28" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="D28" s="65"/>
-      <c r="E28" s="80"/>
-      <c r="F28" s="81"/>
-      <c r="G28" s="52"/>
-      <c r="H28" s="85"/>
-      <c r="I28" s="86"/>
-      <c r="K28" s="44"/>
-      <c r="L28" s="44"/>
-      <c r="M28" s="45"/>
-      <c r="N28" s="23"/>
-      <c r="Y28" s="49"/>
+      <c r="D28" s="64"/>
+      <c r="E28" s="96"/>
+      <c r="F28" s="97"/>
+      <c r="G28" s="51"/>
+      <c r="H28" s="98"/>
+      <c r="I28" s="99"/>
+      <c r="K28" s="43"/>
+      <c r="L28" s="43"/>
+      <c r="M28" s="44"/>
+      <c r="N28" s="22"/>
+      <c r="Y28" s="48"/>
     </row>
     <row r="29" spans="1:25" ht="19.8">
-      <c r="A29" s="39" t="s">
+      <c r="A29" s="38" t="s">
         <v>36</v>
       </c>
-      <c r="B29" s="40"/>
-      <c r="C29" s="41" t="s">
+      <c r="B29" s="39"/>
+      <c r="C29" s="40" t="s">
         <v>37</v>
       </c>
-      <c r="D29" s="65"/>
-      <c r="E29" s="80"/>
-      <c r="F29" s="81"/>
-      <c r="G29" s="52"/>
-      <c r="H29" s="85"/>
-      <c r="I29" s="86"/>
-      <c r="K29" s="44"/>
-      <c r="L29" s="44"/>
-      <c r="M29" s="45"/>
-      <c r="N29" s="23"/>
-      <c r="Y29" s="50"/>
+      <c r="D29" s="64"/>
+      <c r="E29" s="96"/>
+      <c r="F29" s="97"/>
+      <c r="G29" s="51"/>
+      <c r="H29" s="98"/>
+      <c r="I29" s="99"/>
+      <c r="K29" s="43"/>
+      <c r="L29" s="43"/>
+      <c r="M29" s="44"/>
+      <c r="N29" s="22"/>
+      <c r="Y29" s="49"/>
     </row>
     <row r="30" spans="1:25" ht="25.5" customHeight="1">
-      <c r="A30" s="66" t="s">
+      <c r="A30" s="65" t="s">
         <v>38</v>
       </c>
-      <c r="B30" s="82"/>
-      <c r="C30" s="82"/>
-      <c r="D30" s="82"/>
-      <c r="E30" s="82"/>
-      <c r="F30" s="82"/>
-      <c r="G30" s="82"/>
-      <c r="H30" s="67"/>
-      <c r="I30" s="67"/>
-      <c r="Y30" s="50"/>
+      <c r="B30" s="93"/>
+      <c r="C30" s="93"/>
+      <c r="D30" s="93"/>
+      <c r="E30" s="93"/>
+      <c r="F30" s="93"/>
+      <c r="G30" s="93"/>
+      <c r="H30" s="66"/>
+      <c r="I30" s="66"/>
+      <c r="Y30" s="49"/>
     </row>
     <row r="31" spans="1:25" ht="25.5" customHeight="1">
-      <c r="A31" s="66"/>
-      <c r="B31" s="68"/>
-      <c r="C31" s="68"/>
-      <c r="D31" s="68"/>
-      <c r="E31" s="68"/>
-      <c r="F31" s="68"/>
-      <c r="G31" s="68"/>
-      <c r="H31" s="67"/>
-      <c r="I31" s="67"/>
+      <c r="A31" s="65"/>
+      <c r="B31" s="67"/>
+      <c r="C31" s="67"/>
+      <c r="D31" s="67"/>
+      <c r="E31" s="67"/>
+      <c r="F31" s="67"/>
+      <c r="G31" s="67"/>
+      <c r="H31" s="66"/>
+      <c r="I31" s="66"/>
     </row>
     <row r="32" spans="1:25" ht="19.8">
-      <c r="A32" s="69" t="s">
+      <c r="A32" s="68" t="s">
         <v>39</v>
       </c>
-      <c r="B32" s="70"/>
-      <c r="C32" s="70"/>
+      <c r="B32" s="69"/>
+      <c r="C32" s="69"/>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
@@ -1801,9 +1801,9 @@
       <c r="I32" s="1"/>
     </row>
     <row r="33" spans="1:9" ht="19.8">
-      <c r="A33" s="69"/>
-      <c r="B33" s="69"/>
-      <c r="C33" s="69"/>
+      <c r="A33" s="68"/>
+      <c r="B33" s="68"/>
+      <c r="C33" s="68"/>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
@@ -1812,15 +1812,15 @@
       <c r="I33" s="1"/>
     </row>
     <row r="34" spans="1:9" ht="17.399999999999999">
-      <c r="A34" s="71" t="s">
+      <c r="A34" s="70" t="s">
         <v>40</v>
       </c>
-      <c r="B34" s="71"/>
-      <c r="C34" s="71"/>
-      <c r="D34" s="71"/>
-      <c r="E34" s="71"/>
-      <c r="H34" s="72"/>
-      <c r="I34" s="72" t="s">
+      <c r="B34" s="70"/>
+      <c r="C34" s="70"/>
+      <c r="D34" s="70"/>
+      <c r="E34" s="70"/>
+      <c r="H34" s="71"/>
+      <c r="I34" s="71" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1851,15 +1851,11 @@
     <protectedRange sqref="E10" name="Range1_3"/>
   </protectedRanges>
   <mergeCells count="30">
-    <mergeCell ref="E12:H13"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="Y17:Y19"/>
-    <mergeCell ref="A18:C19"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="E18:F19"/>
-    <mergeCell ref="G18:G19"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E29:F29"/>
     <mergeCell ref="B30:G30"/>
     <mergeCell ref="H20:I20"/>
     <mergeCell ref="H21:I21"/>
@@ -1876,11 +1872,15 @@
     <mergeCell ref="E22:F22"/>
     <mergeCell ref="E23:F23"/>
     <mergeCell ref="E24:F24"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="E12:H13"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="Y17:Y19"/>
+    <mergeCell ref="A18:C19"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="E18:F19"/>
+    <mergeCell ref="G18:G19"/>
   </mergeCells>
   <conditionalFormatting sqref="I12:I16 E12 E14:H16">
     <cfRule type="cellIs" dxfId="1" priority="2" stopIfTrue="1" operator="equal">

</xml_diff>